<commit_message>
added a few system test reportsd
</commit_message>
<xml_diff>
--- a/docs/System_Test_Report_template.xlsx
+++ b/docs/System_Test_Report_template.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D795A9-363B-4843-9D23-0103A6759339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overall Test Report" sheetId="2" r:id="rId1"/>
     <sheet name="Test Cases &amp; Results" sheetId="1" r:id="rId2"/>
     <sheet name="Enums" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -20,6 +21,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="83">
   <si>
     <t>Total Test Cases</t>
   </si>
@@ -96,13 +99,199 @@
   </si>
   <si>
     <t>REQ-06</t>
+  </si>
+  <si>
+    <t>REQ-01</t>
+  </si>
+  <si>
+    <t>Test that the LCD shows "Please scan your Identity card" when the system is turned on</t>
+  </si>
+  <si>
+    <t>The system is turned on</t>
+  </si>
+  <si>
+    <t>Provide power to the Raspberry Pi and run the main.py file using python main.py</t>
+  </si>
+  <si>
+    <t>The LCD shows "Please scan your Identity card"</t>
+  </si>
+  <si>
+    <t>REQ-02</t>
+  </si>
+  <si>
+    <t>REQ-03</t>
+  </si>
+  <si>
+    <t>REQ-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test that once the user has scan their card, the Raspberry Pi scans the database for Profiles that match the ID. 
+</t>
+  </si>
+  <si>
+    <t>The user scans a QR code or Barcode with their id String embedded</t>
+  </si>
+  <si>
+    <t>Use a QR code embedded with test account id "P2426082", bring it in front of the PiCam and let it scan</t>
+  </si>
+  <si>
+    <t>Firebase should show that there has been a read command on its activity tracker</t>
+  </si>
+  <si>
+    <t>REQ-05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test that if no match is found in REQ-02 the LCD should Display 
+“No account found” </t>
+  </si>
+  <si>
+    <t>The user scans a QR code or Barcode with a id embedded that is not in the system</t>
+  </si>
+  <si>
+    <t>Use a QR code embedded with invalid account id (Giberrish will work), bring it in front of the PiCam and let it scan</t>
+  </si>
+  <si>
+    <t>The LCD displays "No Account found"</t>
+  </si>
+  <si>
+    <t>Test that if there is a match in REQ-02 the LCD should Display 
+“1 –Collect Books 2- Return Books”</t>
+  </si>
+  <si>
+    <t>The user scans a QR code or Barcode with a id embedded that is in the system</t>
+  </si>
+  <si>
+    <t>Use a QR code embedded with a valid account id: test account is "P2426082", bring it in front of the PiCam and let it scan</t>
+  </si>
+  <si>
+    <t>The LCD displays
+“1 –Collect Books 2- Return Books”</t>
+  </si>
+  <si>
+    <t>Test that in REQ-04 if option 1 is selected on the matrix keypad, REQ-06 is started</t>
+  </si>
+  <si>
+    <t>Check that the database is checked out outstanding fines associated with this account</t>
+  </si>
+  <si>
+    <t>The user selects 1 in the Matrix keypad from REQ-04</t>
+  </si>
+  <si>
+    <t>REQ-07</t>
+  </si>
+  <si>
+    <t>REQ-08</t>
+  </si>
+  <si>
+    <t>REQ-09</t>
+  </si>
+  <si>
+    <t>REQ-10</t>
+  </si>
+  <si>
+    <t>Compare to see if the user has</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Display on LCD "Pls tap card to pay xxx" if the user has a fine </t>
+  </si>
+  <si>
+    <t>User must be fined with any amount of money. User must select collect book on the raspberry pi keypad</t>
+  </si>
+  <si>
+    <t>Assign the account "P2426082" with a fine manually by hand, go through the previous tests and select 1 when asked  in REQ-04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The LCD displays  "Pls tap card to pay xxx" </t>
+  </si>
+  <si>
+    <t>Test that when the user taps his card, the fine is deducted from the card</t>
+  </si>
+  <si>
+    <t>The user must go through REQ-08</t>
+  </si>
+  <si>
+    <t>Fine is deducted from the card and the card balance goes down by the correct amount</t>
+  </si>
+  <si>
+    <t>Test that Firebase updates and clears the account's fine</t>
+  </si>
+  <si>
+    <t>The user must go through REQ-09</t>
+  </si>
+  <si>
+    <t>Follow the same steps as test case 10, no additional steps required</t>
+  </si>
+  <si>
+    <t>The fine amount on Firebase for the test account is set to 0</t>
+  </si>
+  <si>
+    <t>REQ-11</t>
+  </si>
+  <si>
+    <t>Test that if humidity is high, REQ-12 is carried out</t>
+  </si>
+  <si>
+    <t>The humidity must be high at the humidity sensor</t>
+  </si>
+  <si>
+    <t>Place a wet cloth or tissue on the humidity sensor and observe the output</t>
+  </si>
+  <si>
+    <t>REQ-12 is carried out</t>
+  </si>
+  <si>
+    <t>REQ-12</t>
+  </si>
+  <si>
+    <t>Test that if humidity is high, Buzzer is beeped quickly for 3 seconds</t>
+  </si>
+  <si>
+    <t>Humidity must be high at REQ-11</t>
+  </si>
+  <si>
+    <t>Follow the same steps as test case 9 and then tap the RFID card on the reader</t>
+  </si>
+  <si>
+    <t>Buzzer is beeped quickly for 3 seconds</t>
+  </si>
+  <si>
+    <t>REQ-13</t>
+  </si>
+  <si>
+    <t>Test motor is turned on to dispense book after past steps</t>
+  </si>
+  <si>
+    <t>Test that LED is turned on for 3 seconds after humidity is high</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test that LED is turned on for 3 seconds </t>
+  </si>
+  <si>
+    <t xml:space="preserve">One of these must occur
+- Humidity is high and the buzzer and LED has finished
+-Humidity is not high </t>
+  </si>
+  <si>
+    <t>Follow the same steps as test case 13, no additional steps required</t>
+  </si>
+  <si>
+    <t>Follow the same steps as test case 12, no additional steps required</t>
+  </si>
+  <si>
+    <t>Follow the same steps as test case 14, no additional steps required</t>
+  </si>
+  <si>
+    <t>REQ-14</t>
+  </si>
+  <si>
+    <t>Servo Motor turns 90 degrees for a few seconds and returns to its original position</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,6 +310,12 @@
     <font>
       <sz val="9"/>
       <color rgb="FF333333"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
       <name val="Verdana"/>
       <family val="2"/>
     </font>
@@ -190,20 +385,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -221,22 +407,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -248,13 +435,6 @@
       <fill>
         <patternFill>
           <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -274,7 +454,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -311,7 +491,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -487,13 +666,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1208,9 +1387,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1248,9 +1427,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1285,7 +1464,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1320,7 +1499,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1493,52 +1672,52 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:C6"/>
   <sheetViews>
     <sheetView zoomScale="129" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="7">
         <f>COUNTIF('Test Cases &amp; Results'!B3:B70, "&lt;&gt;")</f>
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="7">
         <f>COUNTIF('Test Cases &amp; Results'!K3:K72, "Pass")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="7">
         <f>COUNTIF('Test Cases &amp; Results'!K3:K72, "Fail")</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B6" s="9" t="s">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="7">
         <f>COUNTIF('Test Cases &amp; Results'!K3:K72, "Not Tested")</f>
-        <v>19</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1549,28 +1728,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B2:K71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="136" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="28.140625" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" customWidth="1"/>
-    <col min="8" max="8" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" style="13" customWidth="1"/>
+    <col min="6" max="6" width="28.109375" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" customWidth="1"/>
+    <col min="8" max="8" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.44140625" customWidth="1"/>
+    <col min="10" max="10" width="18.5546875" customWidth="1"/>
+    <col min="11" max="11" width="12.5546875" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1598,11 +1777,11 @@
       <c r="J2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="K2" s="8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:11" ht="57" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2">
         <v>1</v>
       </c>
@@ -1612,370 +1791,1081 @@
       <c r="D3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="J3" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="K3" s="9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11" ht="45.6" x14ac:dyDescent="0.3">
       <c r="B4" s="2">
         <f>B3+1</f>
         <v>2</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" ht="57" x14ac:dyDescent="0.3">
       <c r="B5" s="2">
         <f t="shared" ref="B5:B20" si="0">B4+1</f>
         <v>3</v>
       </c>
       <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="57" x14ac:dyDescent="0.3">
       <c r="B6" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C6" s="13"/>
+      <c r="D6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B7" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C7" s="13"/>
+      <c r="D7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B8" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="12" t="s">
+      <c r="C8" s="13"/>
+      <c r="D8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B9" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="12" t="s">
+      <c r="C9" s="13"/>
+      <c r="D9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="12" t="s">
+      <c r="C10" s="13"/>
+      <c r="D10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C11" s="13"/>
+      <c r="D11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="K11" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" ht="72" x14ac:dyDescent="0.3">
       <c r="B12" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
-      <c r="K12" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C12" s="13"/>
+      <c r="D12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B13" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
-      <c r="K13" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C13" s="13"/>
+      <c r="D13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="K13" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B14" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C14" s="13"/>
+      <c r="D14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="J14" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B15" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
-      <c r="K15" s="12" t="s">
+      <c r="C15" s="13"/>
+      <c r="D15" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="J15" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="K15" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B16" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="12" t="s">
+      <c r="C16" s="13"/>
+      <c r="D16" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="J16" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="K16" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" ht="72" x14ac:dyDescent="0.3">
       <c r="B17" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="12" t="s">
+      <c r="C17" s="13"/>
+      <c r="D17" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="J17" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="K17" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B18" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="12" t="s">
+      <c r="C18" s="13"/>
+      <c r="D18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B19" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="12" t="s">
+      <c r="C19" s="13"/>
+      <c r="D19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B20" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="12" t="s">
+      <c r="C20" s="13"/>
+      <c r="D20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B21" s="2">
         <f t="shared" ref="B21:B22" si="1">B20+1</f>
         <v>19</v>
       </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="12" t="s">
+      <c r="C21" s="13"/>
+      <c r="D21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B22" s="2">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="C22" s="14"/>
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="12" t="s">
+      <c r="C22" s="13"/>
+      <c r="D22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="9" t="s">
         <v>3</v>
       </c>
     </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B23" s="14"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="14"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B26" s="14"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B28" s="14"/>
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
+    </row>
+    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B29" s="14"/>
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B30" s="14"/>
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B31" s="14"/>
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B32" s="14"/>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14"/>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B33" s="14"/>
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="14"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B34" s="14"/>
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="14"/>
+      <c r="J34" s="14"/>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="14"/>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B36" s="14"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B38" s="14"/>
+      <c r="C38" s="14"/>
+      <c r="D38" s="14"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="14"/>
+      <c r="G38" s="14"/>
+      <c r="H38" s="14"/>
+      <c r="I38" s="14"/>
+      <c r="J38" s="14"/>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B39" s="14"/>
+      <c r="C39" s="14"/>
+      <c r="D39" s="14"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="14"/>
+      <c r="G39" s="14"/>
+      <c r="H39" s="14"/>
+      <c r="I39" s="14"/>
+      <c r="J39" s="14"/>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B40" s="14"/>
+      <c r="C40" s="14"/>
+      <c r="D40" s="14"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="14"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="14"/>
+      <c r="I40" s="14"/>
+      <c r="J40" s="14"/>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B41" s="14"/>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+      <c r="G41" s="14"/>
+      <c r="H41" s="14"/>
+      <c r="I41" s="14"/>
+      <c r="J41" s="14"/>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B42" s="14"/>
+      <c r="C42" s="14"/>
+      <c r="D42" s="14"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="14"/>
+      <c r="G42" s="14"/>
+      <c r="H42" s="14"/>
+      <c r="I42" s="14"/>
+      <c r="J42" s="14"/>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="14"/>
+      <c r="I43" s="14"/>
+      <c r="J43" s="14"/>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B44" s="14"/>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="14"/>
+      <c r="H44" s="14"/>
+      <c r="I44" s="14"/>
+      <c r="J44" s="14"/>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B45" s="14"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="14"/>
+      <c r="J45" s="14"/>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B46" s="14"/>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="14"/>
+      <c r="I46" s="14"/>
+      <c r="J46" s="14"/>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B47" s="14"/>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="14"/>
+      <c r="J47" s="14"/>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B48" s="14"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="14"/>
+      <c r="H48" s="14"/>
+      <c r="I48" s="14"/>
+      <c r="J48" s="14"/>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B49" s="14"/>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="14"/>
+      <c r="I49" s="14"/>
+      <c r="J49" s="14"/>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B50" s="14"/>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="14"/>
+      <c r="H50" s="14"/>
+      <c r="I50" s="14"/>
+      <c r="J50" s="14"/>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B51" s="14"/>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="14"/>
+      <c r="H51" s="14"/>
+      <c r="I51" s="14"/>
+      <c r="J51" s="14"/>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B52" s="14"/>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="14"/>
+      <c r="I52" s="14"/>
+      <c r="J52" s="14"/>
+    </row>
+    <row r="53" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B53" s="14"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="14"/>
+      <c r="H53" s="14"/>
+      <c r="I53" s="14"/>
+      <c r="J53" s="14"/>
+    </row>
+    <row r="54" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B54" s="14"/>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="14"/>
+      <c r="H54" s="14"/>
+      <c r="I54" s="14"/>
+      <c r="J54" s="14"/>
+    </row>
+    <row r="55" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B55" s="14"/>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="14"/>
+      <c r="I55" s="14"/>
+      <c r="J55" s="14"/>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B56" s="14"/>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="14"/>
+      <c r="H56" s="14"/>
+      <c r="I56" s="14"/>
+      <c r="J56" s="14"/>
+    </row>
+    <row r="57" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B57" s="14"/>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="14"/>
+      <c r="H57" s="14"/>
+      <c r="I57" s="14"/>
+      <c r="J57" s="14"/>
+    </row>
+    <row r="58" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B58" s="14"/>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="14"/>
+      <c r="H58" s="14"/>
+      <c r="I58" s="14"/>
+      <c r="J58" s="14"/>
+    </row>
+    <row r="59" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B59" s="14"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="14"/>
+      <c r="H59" s="14"/>
+      <c r="I59" s="14"/>
+      <c r="J59" s="14"/>
+    </row>
+    <row r="60" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B60" s="14"/>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="14"/>
+      <c r="H60" s="14"/>
+      <c r="I60" s="14"/>
+      <c r="J60" s="14"/>
+    </row>
+    <row r="61" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B61" s="14"/>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
+      <c r="G61" s="14"/>
+      <c r="H61" s="14"/>
+      <c r="I61" s="14"/>
+      <c r="J61" s="14"/>
+    </row>
+    <row r="62" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B62" s="14"/>
+      <c r="C62" s="14"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14"/>
+      <c r="G62" s="14"/>
+      <c r="H62" s="14"/>
+      <c r="I62" s="14"/>
+      <c r="J62" s="14"/>
+    </row>
+    <row r="63" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B63" s="14"/>
+      <c r="C63" s="14"/>
+      <c r="D63" s="14"/>
+      <c r="E63" s="14"/>
+      <c r="F63" s="14"/>
+      <c r="G63" s="14"/>
+      <c r="H63" s="14"/>
+      <c r="I63" s="14"/>
+      <c r="J63" s="14"/>
+    </row>
+    <row r="64" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B64" s="14"/>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="14"/>
+      <c r="F64" s="14"/>
+      <c r="G64" s="14"/>
+      <c r="H64" s="14"/>
+      <c r="I64" s="14"/>
+      <c r="J64" s="14"/>
+    </row>
+    <row r="65" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B65" s="14"/>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="14"/>
+      <c r="H65" s="14"/>
+      <c r="I65" s="14"/>
+      <c r="J65" s="14"/>
+    </row>
+    <row r="66" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B66" s="14"/>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="14"/>
+      <c r="G66" s="14"/>
+      <c r="H66" s="14"/>
+      <c r="I66" s="14"/>
+      <c r="J66" s="14"/>
+    </row>
+    <row r="67" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B67" s="14"/>
+      <c r="C67" s="14"/>
+      <c r="D67" s="14"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="14"/>
+      <c r="G67" s="14"/>
+      <c r="H67" s="14"/>
+      <c r="I67" s="14"/>
+      <c r="J67" s="14"/>
+    </row>
+    <row r="68" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B68" s="14"/>
+      <c r="C68" s="14"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="14"/>
+      <c r="G68" s="14"/>
+      <c r="H68" s="14"/>
+      <c r="I68" s="14"/>
+      <c r="J68" s="14"/>
+    </row>
+    <row r="69" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B69" s="14"/>
+      <c r="C69" s="14"/>
+      <c r="D69" s="14"/>
+      <c r="E69" s="14"/>
+      <c r="F69" s="14"/>
+      <c r="G69" s="14"/>
+      <c r="H69" s="14"/>
+      <c r="I69" s="14"/>
+      <c r="J69" s="14"/>
+    </row>
+    <row r="70" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B70" s="14"/>
+      <c r="C70" s="14"/>
+      <c r="D70" s="14"/>
+      <c r="E70" s="14"/>
+      <c r="F70" s="14"/>
+      <c r="G70" s="14"/>
+      <c r="H70" s="14"/>
+      <c r="I70" s="14"/>
+      <c r="J70" s="14"/>
+    </row>
+    <row r="71" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B71" s="14"/>
+      <c r="C71" s="14"/>
+      <c r="D71" s="14"/>
+      <c r="E71" s="14"/>
+      <c r="F71" s="14"/>
+      <c r="G71" s="14"/>
+      <c r="H71" s="14"/>
+      <c r="I71" s="14"/>
+      <c r="J71" s="14"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="K3:K20">
-    <cfRule type="cellIs" dxfId="3" priority="9" operator="equal">
-      <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K3:K20">
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
+  <conditionalFormatting sqref="K3:K22">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21:K22">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"Fail"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K21:K22">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"Not Tested"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1983,13 +2873,13 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>Enums!$B$8:$B$10</xm:f>
           </x14:formula1>
           <xm:sqref>E3:E5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>Enums!$B$2:$B$4</xm:f>
           </x14:formula1>
@@ -2002,41 +2892,41 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>17</v>
       </c>
@@ -2048,21 +2938,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E81D8C8DDAE8BD44A422697963F06C45" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b6816e004dbb89c674e51f5647972552">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2b02348f-b4e3-458c-83fc-9e90db0f8029" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e6418ca14ac9ee17b8bbf6df78e0c223" ns2:_="">
     <xsd:import namespace="2b02348f-b4e3-458c-83fc-9e90db0f8029"/>
@@ -2220,31 +3095,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69DB72C7-DF0B-4E18-8174-00AB852E6FB4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2b02348f-b4e3-458c-83fc-9e90db0f8029"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{859B513B-8BED-4B59-B224-E0A2C6173D25}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCDB6385-31B2-4574-9AA4-BF13B563A4E3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2260,4 +3126,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{859B513B-8BED-4B59-B224-E0A2C6173D25}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69DB72C7-DF0B-4E18-8174-00AB852E6FB4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2b02348f-b4e3-458c-83fc-9e90db0f8029"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
REQ-17 and REQ-18 are added to system test report
</commit_message>
<xml_diff>
--- a/docs/System_Test_Report_template.xlsx
+++ b/docs/System_Test_Report_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D795A9-363B-4843-9D23-0103A6759339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86FBFA8-2636-48B2-A824-48A8585A93A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="98">
   <si>
     <t>Total Test Cases</t>
   </si>
@@ -285,6 +285,51 @@
   </si>
   <si>
     <t>Servo Motor turns 90 degrees for a few seconds and returns to its original position</t>
+  </si>
+  <si>
+    <t>REQ-15</t>
+  </si>
+  <si>
+    <t>Test after the servo motor returns to its original position, buzzer is beeped quickly for 3 seconds</t>
+  </si>
+  <si>
+    <t>Servo motor must be back to its original position</t>
+  </si>
+  <si>
+    <t>Follow the same steps as test case 15, no additional steps required</t>
+  </si>
+  <si>
+    <t>REQ-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test that the LCD shows "Please Scan Your Card" after the REQ-15 is completed </t>
+  </si>
+  <si>
+    <t>The buzzer has finished beeping and firebase is updated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Follow the same steps as test case 16, no additional steps required </t>
+  </si>
+  <si>
+    <t>LCD displays "Please Scan Your Card"</t>
+  </si>
+  <si>
+    <t>REQ-17</t>
+  </si>
+  <si>
+    <t>Test that in REQ-04 if option 2 is selected on the matrix keypad, REQ-18 is started</t>
+  </si>
+  <si>
+    <t>REQ-18</t>
+  </si>
+  <si>
+    <t>The user selects 2 in the Matrix keypad from REQ-04</t>
+  </si>
+  <si>
+    <t>LCD displays "Scan book, 0 to end"</t>
+  </si>
+  <si>
+    <t>Test that the LCD shows "Scan book, 0 to end" after option 2 is selected</t>
   </si>
 </sst>
 </file>
@@ -454,7 +499,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1731,8 +1776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:K71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="136" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="D17" zoomScale="136" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2225,55 +2270,83 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B18" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
+        <v>83</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="J18" s="13" t="s">
+        <v>72</v>
+      </c>
       <c r="K18" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B19" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
+        <v>87</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="J19" s="13" t="s">
+        <v>91</v>
+      </c>
       <c r="K19" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B20" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="C20" s="13"/>
       <c r="D20" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
+        <v>92</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>93</v>
+      </c>
       <c r="G20" s="13"/>
       <c r="H20" s="13"/>
       <c r="I20" s="13"/>
@@ -2282,21 +2355,31 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B21" s="2">
         <f t="shared" ref="B21:B22" si="1">B20+1</f>
         <v>19</v>
       </c>
       <c r="C21" s="13"/>
       <c r="D21" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
+        <v>94</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>95</v>
+      </c>
       <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
+      <c r="I21" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="J21" s="13" t="s">
+        <v>96</v>
+      </c>
       <c r="K21" s="9" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
REQ-19 and REQ-20 are added to system test report
</commit_message>
<xml_diff>
--- a/docs/System_Test_Report_template.xlsx
+++ b/docs/System_Test_Report_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86FBFA8-2636-48B2-A824-48A8585A93A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E748DAC-A732-4754-8B29-63315349E85A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="107">
   <si>
     <t>Total Test Cases</t>
   </si>
@@ -330,13 +330,40 @@
   </si>
   <si>
     <t>Test that the LCD shows "Scan book, 0 to end" after option 2 is selected</t>
+  </si>
+  <si>
+    <t>REQ-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test whether user enter 0 from matrix keypad </t>
+  </si>
+  <si>
+    <t>REQ-20</t>
+  </si>
+  <si>
+    <t>The user must go through REQ-18</t>
+  </si>
+  <si>
+    <t>From the LCD main menu from REQ-18, enter 0</t>
+  </si>
+  <si>
+    <t>If the 0 is pressed, REQ-29 is carried out, otherwise it continues to REQ-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test if the barcode has been scanned </t>
+  </si>
+  <si>
+    <t>The user must not press 0 in REQ-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The scanned QR code is later used to calculate fine and let the system proceeds to REQ-21 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -363,6 +390,12 @@
       <color theme="1"/>
       <name val="Verdana"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -717,7 +750,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1735,7 +1768,7 @@
       </c>
       <c r="C3" s="7">
         <f>COUNTIF('Test Cases &amp; Results'!B3:B70, "&lt;&gt;")</f>
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
@@ -1762,7 +1795,7 @@
       </c>
       <c r="C6" s="7">
         <f>COUNTIF('Test Cases &amp; Results'!K3:K72, "Not Tested")</f>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1776,8 +1809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:K71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D17" zoomScale="136" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="136" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2357,7 +2390,7 @@
     </row>
     <row r="21" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B21" s="2">
-        <f t="shared" ref="B21:B22" si="1">B20+1</f>
+        <f t="shared" ref="B21:B23" si="1">B20+1</f>
         <v>19</v>
       </c>
       <c r="C21" s="13"/>
@@ -2384,35 +2417,67 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B22" s="2">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C22" s="13"/>
       <c r="D22" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
+        <v>98</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="J22" s="13" t="s">
+        <v>103</v>
+      </c>
       <c r="K22" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
+    <row r="23" spans="2:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="B23" s="2">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="J23" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="K23" s="9" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B24" s="14"/>
@@ -2943,7 +3008,8 @@
       <c r="J71" s="14"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="K3:K22">
+  <phoneticPr fontId="4" type="noConversion"/>
+  <conditionalFormatting sqref="K3:K23">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
@@ -2966,7 +3032,7 @@
           <x14:formula1>
             <xm:f>Enums!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>K3:K22</xm:sqref>
+          <xm:sqref>K3:K23</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3021,6 +3087,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E81D8C8DDAE8BD44A422697963F06C45" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b6816e004dbb89c674e51f5647972552">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2b02348f-b4e3-458c-83fc-9e90db0f8029" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e6418ca14ac9ee17b8bbf6df78e0c223" ns2:_="">
     <xsd:import namespace="2b02348f-b4e3-458c-83fc-9e90db0f8029"/>
@@ -3178,22 +3259,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69DB72C7-DF0B-4E18-8174-00AB852E6FB4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2b02348f-b4e3-458c-83fc-9e90db0f8029"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{859B513B-8BED-4B59-B224-E0A2C6173D25}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCDB6385-31B2-4574-9AA4-BF13B563A4E3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3209,28 +3299,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{859B513B-8BED-4B59-B224-E0A2C6173D25}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69DB72C7-DF0B-4E18-8174-00AB852E6FB4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2b02348f-b4e3-458c-83fc-9e90db0f8029"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
REQ-21 and REQ-22 are added to system test report
</commit_message>
<xml_diff>
--- a/docs/System_Test_Report_template.xlsx
+++ b/docs/System_Test_Report_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E748DAC-A732-4754-8B29-63315349E85A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5748D0F4-9B02-4896-B275-674E1F3393C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="113">
   <si>
     <t>Total Test Cases</t>
   </si>
@@ -357,6 +357,24 @@
   </si>
   <si>
     <t xml:space="preserve">The scanned QR code is later used to calculate fine and let the system proceeds to REQ-21 </t>
+  </si>
+  <si>
+    <t>REQ-21</t>
+  </si>
+  <si>
+    <t>REQ-22</t>
+  </si>
+  <si>
+    <t>Test that if humidity is high, REQ-22 is carried out</t>
+  </si>
+  <si>
+    <t>Humidity must be high at humidity sensor</t>
+  </si>
+  <si>
+    <t>REQ-22 is carried out</t>
+  </si>
+  <si>
+    <t>Humidity must be high at REQ-21</t>
   </si>
 </sst>
 </file>
@@ -750,7 +768,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1768,7 +1786,7 @@
       </c>
       <c r="C3" s="7">
         <f>COUNTIF('Test Cases &amp; Results'!B3:B70, "&lt;&gt;")</f>
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
@@ -1795,7 +1813,7 @@
       </c>
       <c r="C6" s="7">
         <f>COUNTIF('Test Cases &amp; Results'!K3:K72, "Not Tested")</f>
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -1809,7 +1827,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:K71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="136" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D22" zoomScale="136" workbookViewId="0">
       <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
@@ -2390,7 +2408,7 @@
     </row>
     <row r="21" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B21" s="2">
-        <f t="shared" ref="B21:B23" si="1">B20+1</f>
+        <f t="shared" ref="B21:B25" si="1">B20+1</f>
         <v>19</v>
       </c>
       <c r="C21" s="13"/>
@@ -2479,27 +2497,67 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
+    <row r="24" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B24" s="2">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="C24" s="13"/>
+      <c r="D24" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="J24" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="K24" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B25" s="2">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="C25" s="13"/>
+      <c r="D25" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="J25" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="K25" s="9" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B26" s="14"/>
@@ -3009,7 +3067,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="K3:K23">
+  <conditionalFormatting sqref="K3:K25">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
@@ -3032,7 +3090,7 @@
           <x14:formula1>
             <xm:f>Enums!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>K3:K23</xm:sqref>
+          <xm:sqref>K3:K25</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3087,21 +3145,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E81D8C8DDAE8BD44A422697963F06C45" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b6816e004dbb89c674e51f5647972552">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2b02348f-b4e3-458c-83fc-9e90db0f8029" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e6418ca14ac9ee17b8bbf6df78e0c223" ns2:_="">
     <xsd:import namespace="2b02348f-b4e3-458c-83fc-9e90db0f8029"/>
@@ -3259,31 +3302,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69DB72C7-DF0B-4E18-8174-00AB852E6FB4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2b02348f-b4e3-458c-83fc-9e90db0f8029"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{859B513B-8BED-4B59-B224-E0A2C6173D25}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCDB6385-31B2-4574-9AA4-BF13B563A4E3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3299,4 +3333,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{859B513B-8BED-4B59-B224-E0A2C6173D25}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69DB72C7-DF0B-4E18-8174-00AB852E6FB4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2b02348f-b4e3-458c-83fc-9e90db0f8029"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
REQ-23 and REQ-24 are added to system test report
</commit_message>
<xml_diff>
--- a/docs/System_Test_Report_template.xlsx
+++ b/docs/System_Test_Report_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5748D0F4-9B02-4896-B275-674E1F3393C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2048BFBB-8C83-4CA4-83CE-9857B7AB07FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="120">
   <si>
     <t>Total Test Cases</t>
   </si>
@@ -375,6 +375,27 @@
   </si>
   <si>
     <t>Humidity must be high at REQ-21</t>
+  </si>
+  <si>
+    <t>REQ-23</t>
+  </si>
+  <si>
+    <t>REQ-24</t>
+  </si>
+  <si>
+    <t>Follow the same steps as test case 22, no additional steps required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED is turned on for 3 seconds </t>
+  </si>
+  <si>
+    <t>Test that if the return date is late or not by checking from firebase data</t>
+  </si>
+  <si>
+    <t>The user must scan in REQ-20</t>
+  </si>
+  <si>
+    <t>The return date is correctly calculated in returnbooks function in main.py</t>
   </si>
 </sst>
 </file>
@@ -768,7 +789,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1786,7 +1807,7 @@
       </c>
       <c r="C3" s="7">
         <f>COUNTIF('Test Cases &amp; Results'!B3:B70, "&lt;&gt;")</f>
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
@@ -1813,7 +1834,7 @@
       </c>
       <c r="C6" s="7">
         <f>COUNTIF('Test Cases &amp; Results'!K3:K72, "Not Tested")</f>
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1827,8 +1848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:K71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D22" zoomScale="136" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="136" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2408,7 +2429,7 @@
     </row>
     <row r="21" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B21" s="2">
-        <f t="shared" ref="B21:B25" si="1">B20+1</f>
+        <f t="shared" ref="B21:B27" si="1">B20+1</f>
         <v>19</v>
       </c>
       <c r="C21" s="13"/>
@@ -2547,7 +2568,7 @@
         <v>112</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>79</v>
+        <v>115</v>
       </c>
       <c r="I25" s="13" t="s">
         <v>72</v>
@@ -2559,27 +2580,65 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B26" s="14"/>
+    <row r="26" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B26" s="2">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
       <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B27" s="14"/>
+      <c r="D26" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="J26" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="K26" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B27" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
       <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
+      <c r="D27" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="J27" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="K27" s="9" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B28" s="14"/>
@@ -3067,7 +3126,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="K3:K25">
+  <conditionalFormatting sqref="K3:K27">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
@@ -3090,7 +3149,7 @@
           <x14:formula1>
             <xm:f>Enums!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>K3:K25</xm:sqref>
+          <xm:sqref>K3:K27</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
REQ-25 and REQ-26 are added to system test report
</commit_message>
<xml_diff>
--- a/docs/System_Test_Report_template.xlsx
+++ b/docs/System_Test_Report_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2048BFBB-8C83-4CA4-83CE-9857B7AB07FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC7B80A-2623-4A40-B38D-29E501C0873D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="127">
   <si>
     <t>Total Test Cases</t>
   </si>
@@ -392,10 +392,31 @@
     <t>Test that if the return date is late or not by checking from firebase data</t>
   </si>
   <si>
-    <t>The user must scan in REQ-20</t>
-  </si>
-  <si>
-    <t>The return date is correctly calculated in returnbooks function in main.py</t>
+    <t>REQ-25</t>
+  </si>
+  <si>
+    <t>REQ-26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test book loan date from firebase </t>
+  </si>
+  <si>
+    <t>The bookloan date is correctly retreived in returnbooks function in main.py</t>
+  </si>
+  <si>
+    <t>The user must scan the barcode in REQ-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The return date is correctly calculated in returnbooks function in main.py and proceeds to REQ-26 or 27 </t>
+  </si>
+  <si>
+    <t>Test the calculation of fine amount that need to be paid</t>
+  </si>
+  <si>
+    <t>The return date must be considered late from REQ-25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test account in database is updated with additional fine </t>
   </si>
 </sst>
 </file>
@@ -789,7 +810,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1807,7 +1828,7 @@
       </c>
       <c r="C3" s="7">
         <f>COUNTIF('Test Cases &amp; Results'!B3:B70, "&lt;&gt;")</f>
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
@@ -1834,7 +1855,7 @@
       </c>
       <c r="C6" s="7">
         <f>COUNTIF('Test Cases &amp; Results'!K3:K72, "Not Tested")</f>
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1848,8 +1869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:K71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" zoomScale="136" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" topLeftCell="B25" zoomScale="136" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2429,7 +2450,7 @@
     </row>
     <row r="21" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B21" s="2">
-        <f t="shared" ref="B21:B27" si="1">B20+1</f>
+        <f t="shared" ref="B21:B29" si="1">B20+1</f>
         <v>19</v>
       </c>
       <c r="C21" s="13"/>
@@ -2624,43 +2645,79 @@
         <v>16</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="G27" s="13" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="H27" s="13"/>
       <c r="I27" s="13" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="J27" s="13" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="K27" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B28" s="14"/>
+    <row r="28" spans="2:11" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B28" s="2">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
       <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B29" s="14"/>
+      <c r="D28" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="J28" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="K28" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B29" s="2">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
       <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
+      <c r="D29" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="J29" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="K29" s="9" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B30" s="14"/>
@@ -2669,7 +2726,6 @@
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
       <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
       <c r="I30" s="14"/>
       <c r="J30" s="14"/>
     </row>
@@ -2680,7 +2736,6 @@
       <c r="E31" s="14"/>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
       <c r="I31" s="14"/>
       <c r="J31" s="14"/>
     </row>
@@ -3126,7 +3181,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="K3:K27">
+  <conditionalFormatting sqref="K3:K29">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
@@ -3149,7 +3204,7 @@
           <x14:formula1>
             <xm:f>Enums!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>K3:K27</xm:sqref>
+          <xm:sqref>K3:K29</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
REQ-27, REQ-28 and REQ-29 are added to system test report
</commit_message>
<xml_diff>
--- a/docs/System_Test_Report_template.xlsx
+++ b/docs/System_Test_Report_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECC7B80A-2623-4A40-B38D-29E501C0873D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7ABD0D2-2D75-4E9C-9EF4-E5DF157540E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="139">
   <si>
     <t>Total Test Cases</t>
   </si>
@@ -417,6 +417,42 @@
   </si>
   <si>
     <t xml:space="preserve">Test account in database is updated with additional fine </t>
+  </si>
+  <si>
+    <t>REQ-27</t>
+  </si>
+  <si>
+    <t>REQ-28</t>
+  </si>
+  <si>
+    <t>REQ-29</t>
+  </si>
+  <si>
+    <t>Test if the loan status of the account in firebase is removed</t>
+  </si>
+  <si>
+    <t>The return date must not be considered late from REQ-26</t>
+  </si>
+  <si>
+    <t>Loan status of the test account in database is removed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test that LCD shows the confirmation messeage after the loan status is removed </t>
+  </si>
+  <si>
+    <t>The user must go through REQ-27</t>
+  </si>
+  <si>
+    <t>LCD shows the confirmation message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test that the LCD shows "Please Scan Your Card" after the REQ-28 is completed </t>
+  </si>
+  <si>
+    <t>The firebase is updated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Follow the same steps as test case 29, no additional steps required </t>
   </si>
 </sst>
 </file>
@@ -810,7 +846,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1828,7 +1864,7 @@
       </c>
       <c r="C3" s="7">
         <f>COUNTIF('Test Cases &amp; Results'!B3:B70, "&lt;&gt;")</f>
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
@@ -1855,7 +1891,7 @@
       </c>
       <c r="C6" s="7">
         <f>COUNTIF('Test Cases &amp; Results'!K3:K72, "Not Tested")</f>
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1869,8 +1905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:K71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" zoomScale="136" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="136" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2450,7 +2486,7 @@
     </row>
     <row r="21" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B21" s="2">
-        <f t="shared" ref="B21:B29" si="1">B20+1</f>
+        <f t="shared" ref="B21:B32" si="1">B20+1</f>
         <v>19</v>
       </c>
       <c r="C21" s="13"/>
@@ -2719,36 +2755,94 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B30" s="14"/>
+    <row r="30" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B30" s="2">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
       <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B31" s="14"/>
+      <c r="D30" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="J30" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="K30" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B31" s="2">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
       <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B32" s="14"/>
+      <c r="D31" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="J31" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="K31" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B32" s="2">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
       <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
+      <c r="D32" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="I32" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="J32" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="K32" s="9" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B33" s="14"/>
@@ -3181,7 +3275,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="K3:K29">
+  <conditionalFormatting sqref="K3:K32">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
@@ -3204,7 +3298,7 @@
           <x14:formula1>
             <xm:f>Enums!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>K3:K29</xm:sqref>
+          <xm:sqref>K3:K32</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Merged into 1 commit as i somehow cooked my local proj folder: SYstem test till req34 and moved some SRS id
</commit_message>
<xml_diff>
--- a/docs/System_Test_Report_template.xlsx
+++ b/docs/System_Test_Report_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D795A9-363B-4843-9D23-0103A6759339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEB041A-E3BB-44D2-AA2A-0D595A2EDE60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="204">
   <si>
     <t>Total Test Cases</t>
   </si>
@@ -187,9 +187,6 @@
   </si>
   <si>
     <t>REQ-10</t>
-  </si>
-  <si>
-    <t>Compare to see if the user has</t>
   </si>
   <si>
     <t xml:space="preserve">Display on LCD "Pls tap card to pay xxx" if the user has a fine </t>
@@ -285,13 +282,381 @@
   </si>
   <si>
     <t>Servo Motor turns 90 degrees for a few seconds and returns to its original position</t>
+  </si>
+  <si>
+    <t>REQ-15</t>
+  </si>
+  <si>
+    <t>Test after the servo motor returns to its original position, buzzer is beeped quickly for 3 seconds</t>
+  </si>
+  <si>
+    <t>Servo motor must be back to its original position</t>
+  </si>
+  <si>
+    <t>Follow the same steps as test case 15, no additional steps required</t>
+  </si>
+  <si>
+    <t>REQ-16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test that the LCD shows "Please Scan Your Card" after the REQ-15 is completed </t>
+  </si>
+  <si>
+    <t>The buzzer has finished beeping and firebase is updated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Follow the same steps as test case 16, no additional steps required </t>
+  </si>
+  <si>
+    <t>LCD displays "Please Scan Your Card"</t>
+  </si>
+  <si>
+    <t>REQ-17</t>
+  </si>
+  <si>
+    <t>Test that in REQ-04 if option 2 is selected on the matrix keypad, REQ-18 is started</t>
+  </si>
+  <si>
+    <t>REQ-18</t>
+  </si>
+  <si>
+    <t>The user selects 2 in the Matrix keypad from REQ-04</t>
+  </si>
+  <si>
+    <t>LCD displays "Scan book, 0 to end"</t>
+  </si>
+  <si>
+    <t>Test that the LCD shows "Scan book, 0 to end" after option 2 is selected</t>
+  </si>
+  <si>
+    <t>REQ-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test whether user enter 0 from matrix keypad </t>
+  </si>
+  <si>
+    <t>REQ-20</t>
+  </si>
+  <si>
+    <t>The user must go through REQ-18</t>
+  </si>
+  <si>
+    <t>From the LCD main menu from REQ-18, enter 0</t>
+  </si>
+  <si>
+    <t>If the 0 is pressed, REQ-29 is carried out, otherwise it continues to REQ-20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test if the barcode has been scanned </t>
+  </si>
+  <si>
+    <t>The user must not press 0 in REQ-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The scanned QR code is later used to calculate fine and let the system proceeds to REQ-21 </t>
+  </si>
+  <si>
+    <t>REQ-21</t>
+  </si>
+  <si>
+    <t>REQ-22</t>
+  </si>
+  <si>
+    <t>Test that if humidity is high, REQ-22 is carried out</t>
+  </si>
+  <si>
+    <t>Humidity must be high at humidity sensor</t>
+  </si>
+  <si>
+    <t>Humidity must be high at REQ-21</t>
+  </si>
+  <si>
+    <t>REQ-23</t>
+  </si>
+  <si>
+    <t>REQ-24</t>
+  </si>
+  <si>
+    <t>Follow the same steps as test case 22, no additional steps required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED is turned on for 3 seconds </t>
+  </si>
+  <si>
+    <t>Test that if the return date is late or not by checking from firebase data</t>
+  </si>
+  <si>
+    <t>REQ-25</t>
+  </si>
+  <si>
+    <t>REQ-26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test book loan date from firebase </t>
+  </si>
+  <si>
+    <t>The user must scan the barcode in REQ-20</t>
+  </si>
+  <si>
+    <t>Test the calculation of fine amount that need to be paid</t>
+  </si>
+  <si>
+    <t>The return date must be considered late from REQ-25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test account in database is updated with additional fine </t>
+  </si>
+  <si>
+    <t>REQ-27</t>
+  </si>
+  <si>
+    <t>REQ-28</t>
+  </si>
+  <si>
+    <t>REQ-29</t>
+  </si>
+  <si>
+    <t>Test if the loan status of the account in firebase is removed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test that LCD shows the confirmation messeage after the loan status is removed </t>
+  </si>
+  <si>
+    <t>The user must go through REQ-27</t>
+  </si>
+  <si>
+    <t>LCD shows the confirmation message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test that the LCD shows "Please Scan Your Card" after the REQ-28 is completed </t>
+  </si>
+  <si>
+    <t>The firebase is updated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Follow the same steps as test case 29, no additional steps required </t>
+  </si>
+  <si>
+    <t>Compare to see if the user has fine</t>
+  </si>
+  <si>
+    <t>QR code must be detected by picam</t>
+  </si>
+  <si>
+    <t>After REQ-04 1 must be pressed on keypad</t>
+  </si>
+  <si>
+    <t>The LCD should display something else according to other REQ</t>
+  </si>
+  <si>
+    <t>Manually associate an account "P2426082"with a fine 1 must be pressed on keypad then</t>
+  </si>
+  <si>
+    <t>REQ-08 will be carried out</t>
+  </si>
+  <si>
+    <t>REQ-08 is carried out</t>
+  </si>
+  <si>
+    <t>REQ-06 must be successful</t>
+  </si>
+  <si>
+    <t>Manually associate an account "P2426082"with a fine 1 must be pressed on keypad. Then clear the fine and redo</t>
+  </si>
+  <si>
+    <t>REQ-08 will be carried out first, then REQ-11 for part 2</t>
+  </si>
+  <si>
+    <t>System must be started and QR code must be scanned</t>
+  </si>
+  <si>
+    <t>Start the system, Scan a QR code embedded with "P2426082" and then press 2</t>
+  </si>
+  <si>
+    <t>REQ-18 Is carried out</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The fine is calculated and added to Firebase </t>
+  </si>
+  <si>
+    <t>Chang a book return date back 1 month then
+Follow the same steps as test case 22, no additional steps required</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The bookloan date is correctly retreived and a fine shows up in REQ-25 </t>
+  </si>
+  <si>
+    <t>The user must scan the barcode in REQ-20 and go through the past steps</t>
+  </si>
+  <si>
+    <t>Loan status of the test book in database is removed</t>
+  </si>
+  <si>
+    <t>Change a book return date back 1 month then
+Follow the same steps as test case 22, no additional steps required</t>
+  </si>
+  <si>
+    <t>Go through past steps to loan a book then scan the qr code embedded with the loan book ID in REQ-20</t>
+  </si>
+  <si>
+    <t>REQ-30</t>
+  </si>
+  <si>
+    <t>REQ-31</t>
+  </si>
+  <si>
+    <t>REQ-32</t>
+  </si>
+  <si>
+    <t>REQ-33</t>
+  </si>
+  <si>
+    <t>REQ-34</t>
+  </si>
+  <si>
+    <t>REQ-35</t>
+  </si>
+  <si>
+    <t>REQ-36</t>
+  </si>
+  <si>
+    <t>REQ-37</t>
+  </si>
+  <si>
+    <t>REQ-38</t>
+  </si>
+  <si>
+    <t>REQ-39</t>
+  </si>
+  <si>
+    <t>REQ-40</t>
+  </si>
+  <si>
+    <t>REQ-41</t>
+  </si>
+  <si>
+    <t>REQ-42</t>
+  </si>
+  <si>
+    <t>REQ-43</t>
+  </si>
+  <si>
+    <t>REQ-44</t>
+  </si>
+  <si>
+    <t>REQ-45</t>
+  </si>
+  <si>
+    <t>REQ-46</t>
+  </si>
+  <si>
+    <t>REQ-47</t>
+  </si>
+  <si>
+    <t>REQ-48</t>
+  </si>
+  <si>
+    <t>REQ-49</t>
+  </si>
+  <si>
+    <t>REQ-50</t>
+  </si>
+  <si>
+    <t>REQ-51</t>
+  </si>
+  <si>
+    <t>REQ-52</t>
+  </si>
+  <si>
+    <t>REQ-53</t>
+  </si>
+  <si>
+    <t>REQ-54</t>
+  </si>
+  <si>
+    <t>REQ-55</t>
+  </si>
+  <si>
+    <t>REQ-56</t>
+  </si>
+  <si>
+    <t>REQ-57</t>
+  </si>
+  <si>
+    <t>REQ-58</t>
+  </si>
+  <si>
+    <t>REQ-59</t>
+  </si>
+  <si>
+    <t>REQ-60</t>
+  </si>
+  <si>
+    <t>REQ-61</t>
+  </si>
+  <si>
+    <t>REQ-62</t>
+  </si>
+  <si>
+    <t>REQ-63</t>
+  </si>
+  <si>
+    <t>REQ-64</t>
+  </si>
+  <si>
+    <t>REQ-65</t>
+  </si>
+  <si>
+    <t>REQ-66</t>
+  </si>
+  <si>
+    <t>REQ-67</t>
+  </si>
+  <si>
+    <t>Test that App shall prompt user to input id and password or create an account if they haven’t</t>
+  </si>
+  <si>
+    <t>App must be installed</t>
+  </si>
+  <si>
+    <t>Open the app and press the "New to NLB? Sign Up!" text</t>
+  </si>
+  <si>
+    <t>Rediect to sign up screen where user can input details</t>
+  </si>
+  <si>
+    <t>Test that App shall prompt the user to scan Barcode using camera to get their id</t>
+  </si>
+  <si>
+    <t>App must be installed and app permissions to camera must be given</t>
+  </si>
+  <si>
+    <t>Open the app and press the "New to NLB? Sign Up!" text and press the camera button in the id text field then scan the id barcode</t>
+  </si>
+  <si>
+    <t>Camera scans the barcode and id is auto inputted into the textfield</t>
+  </si>
+  <si>
+    <t>Test that If user enter password in REQ-30 App shall check firebase for matching id and password</t>
+  </si>
+  <si>
+    <t>Open the app and input the adm field "P2426082" and password "123"</t>
+  </si>
+  <si>
+    <t>App redirects to main page</t>
+  </si>
+  <si>
+    <t>Test that If match found in REQ-31 App shall let user into app</t>
+  </si>
+  <si>
+    <t>App must be installed and account is created</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -318,6 +683,12 @@
       <color theme="1"/>
       <name val="Verdana"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -358,7 +729,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -381,11 +752,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -417,6 +803,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -672,7 +1061,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11</c:v>
+                  <c:v>78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1689,8 +2078,8 @@
         <v>0</v>
       </c>
       <c r="C3" s="7">
-        <f>COUNTIF('Test Cases &amp; Results'!B3:B70, "&lt;&gt;")</f>
-        <v>20</v>
+        <f>COUNTIF('Test Cases &amp; Results'!B3:B127, "&lt;&gt;")</f>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="2:3" x14ac:dyDescent="0.3">
@@ -1698,7 +2087,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="7">
-        <f>COUNTIF('Test Cases &amp; Results'!K3:K72, "Pass")</f>
+        <f>COUNTIF('Test Cases &amp; Results'!K3:K129, "Pass")</f>
         <v>9</v>
       </c>
     </row>
@@ -1707,7 +2096,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="7">
-        <f>COUNTIF('Test Cases &amp; Results'!K3:K72, "Fail")</f>
+        <f>COUNTIF('Test Cases &amp; Results'!K3:K129, "Fail")</f>
         <v>0</v>
       </c>
     </row>
@@ -1716,8 +2105,8 @@
         <v>3</v>
       </c>
       <c r="C6" s="7">
-        <f>COUNTIF('Test Cases &amp; Results'!K3:K72, "Not Tested")</f>
-        <v>11</v>
+        <f>COUNTIF('Test Cases &amp; Results'!K3:K129, "Not Tested")</f>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1729,10 +2118,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="B2:K71"/>
+  <dimension ref="B2:K128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="136" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1952,15 +2341,21 @@
       <c r="F8" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="G8" s="13"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
+      <c r="G8" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>136</v>
+      </c>
       <c r="J8" s="13"/>
       <c r="K8" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B9" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1978,14 +2373,20 @@
       <c r="G9" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
+      <c r="H9" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>139</v>
+      </c>
       <c r="K9" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" ht="72" x14ac:dyDescent="0.3">
       <c r="B10" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1998,11 +2399,17 @@
         <v>16</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
-      <c r="I10" s="13"/>
+        <v>133</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>142</v>
+      </c>
       <c r="J10" s="13"/>
       <c r="K10" s="9" t="s">
         <v>3</v>
@@ -2021,19 +2428,19 @@
         <v>17</v>
       </c>
       <c r="F11" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="H11" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="H11" s="13" t="s">
+      <c r="I11" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="I11" s="13" t="s">
-        <v>55</v>
-      </c>
       <c r="J11" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K11" s="9" t="s">
         <v>14</v>
@@ -2052,19 +2459,19 @@
         <v>16</v>
       </c>
       <c r="F12" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="G12" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="H12" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="I12" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="H12" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>58</v>
-      </c>
       <c r="J12" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K12" s="9" t="s">
         <v>14</v>
@@ -2083,19 +2490,19 @@
         <v>16</v>
       </c>
       <c r="F13" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="H13" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="H13" s="13" t="s">
+      <c r="I13" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="I13" s="13" t="s">
-        <v>62</v>
-      </c>
       <c r="J13" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K13" s="9" t="s">
         <v>14</v>
@@ -2108,25 +2515,25 @@
       </c>
       <c r="C14" s="13"/>
       <c r="D14" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E14" s="13" t="s">
         <v>13</v>
       </c>
       <c r="F14" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="H14" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="H14" s="13" t="s">
+      <c r="I14" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="I14" s="13" t="s">
-        <v>67</v>
-      </c>
       <c r="J14" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K14" s="9" t="s">
         <v>14</v>
@@ -2139,25 +2546,25 @@
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E15" s="13" t="s">
         <v>17</v>
       </c>
       <c r="F15" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="G15" s="13" t="s">
-        <v>70</v>
-      </c>
       <c r="H15" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J15" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K15" s="9" t="s">
         <v>3</v>
@@ -2170,25 +2577,25 @@
       </c>
       <c r="C16" s="13"/>
       <c r="D16" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E16" s="13" t="s">
         <v>17</v>
       </c>
       <c r="F16" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="I16" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="G16" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="H16" s="13" t="s">
-        <v>78</v>
-      </c>
-      <c r="I16" s="13" t="s">
-        <v>76</v>
-      </c>
       <c r="J16" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K16" s="9" t="s">
         <v>3</v>
@@ -2201,666 +2608,1928 @@
       </c>
       <c r="C17" s="13"/>
       <c r="D17" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E17" s="13" t="s">
         <v>16</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K17" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B18" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="C18" s="13"/>
       <c r="D18" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
+        <v>82</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="H18" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="J18" s="13" t="s">
+        <v>71</v>
+      </c>
       <c r="K18" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B19" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="C19" s="13"/>
       <c r="D19" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
+        <v>86</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="H19" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="J19" s="13" t="s">
+        <v>90</v>
+      </c>
       <c r="K19" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B20" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="C20" s="13"/>
       <c r="D20" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
+        <v>91</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="H20" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="I20" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="J20" s="13" t="s">
+        <v>95</v>
+      </c>
       <c r="K20" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B21" s="2">
-        <f t="shared" ref="B21:B22" si="1">B20+1</f>
+        <f t="shared" ref="B21:B31" si="1">B20+1</f>
         <v>19</v>
       </c>
       <c r="C21" s="13"/>
       <c r="D21" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
+        <v>93</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="J21" s="13" t="s">
+        <v>95</v>
+      </c>
       <c r="K21" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B22" s="2">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="C22" s="13"/>
       <c r="D22" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E22" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="G22" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="H22" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="J22" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="K22" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="B23" s="2">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="G23" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="J23" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="K23" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B24" s="2">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="C24" s="13"/>
+      <c r="D24" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="G24" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="H24" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="I24" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="J24" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="K24" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B25" s="2">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="C25" s="13"/>
+      <c r="D25" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="H25" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="I25" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="J25" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="K25" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B26" s="2">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="C26" s="14"/>
+      <c r="D26" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="G26" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="H26" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="J26" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="K26" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="2:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="B27" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="C27" s="14"/>
+      <c r="D27" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E27" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="H27" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="I27" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="J27" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="K27" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="2:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="B28" s="2">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E28" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="H28" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="I28" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="J28" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="K28" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="B29" s="2">
+        <f>B28+1</f>
+        <v>27</v>
+      </c>
+      <c r="C29" s="14"/>
+      <c r="D29" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="H29" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="I29" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="J29" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="K29" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B30" s="2">
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="13"/>
-      <c r="H22" s="13"/>
-      <c r="I22" s="13"/>
-      <c r="J22" s="13"/>
-      <c r="K22" s="9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B23" s="14"/>
-      <c r="C23" s="14"/>
-      <c r="D23" s="14"/>
-      <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B24" s="14"/>
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
-      <c r="E24" s="14"/>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
-    </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B25" s="14"/>
-      <c r="C25" s="14"/>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14"/>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
-    </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B26" s="14"/>
-      <c r="C26" s="14"/>
-      <c r="D26" s="14"/>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-    </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
-    </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B28" s="14"/>
-      <c r="C28" s="14"/>
-      <c r="D28" s="14"/>
-      <c r="E28" s="14"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="14"/>
-      <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
-    </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="14"/>
-      <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
-    </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B30" s="14"/>
       <c r="C30" s="14"/>
-      <c r="D30" s="14"/>
-      <c r="E30" s="14"/>
-      <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="14"/>
-      <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
-    </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B31" s="14"/>
+      <c r="D30" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E30" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="I30" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="J30" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="K30" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B31" s="2">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
       <c r="C31" s="14"/>
-      <c r="D31" s="14"/>
-      <c r="E31" s="14"/>
-      <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="14"/>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14"/>
-    </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
-      <c r="B32" s="14"/>
+      <c r="D31" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="H31" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="I31" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="J31" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="K31" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B32" s="2">
+        <v>30</v>
+      </c>
       <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B33" s="14"/>
+      <c r="D32" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="I32" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="J32" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="K32" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="2">
+        <v>31</v>
+      </c>
       <c r="C33" s="14"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="14"/>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14"/>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B34" s="14"/>
+      <c r="D33" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="I33" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="J33" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="K33" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="2">
+        <v>32</v>
+      </c>
       <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="14"/>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B35" s="14"/>
+      <c r="D34" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" s="15" t="s">
+        <v>195</v>
+      </c>
+      <c r="G34" s="13" t="s">
+        <v>196</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="I34" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="J34" s="13" t="s">
+        <v>198</v>
+      </c>
+      <c r="K34" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="2">
+        <v>33</v>
+      </c>
       <c r="C35" s="14"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="14"/>
-      <c r="I35" s="14"/>
-      <c r="J35" s="14"/>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B36" s="14"/>
+      <c r="D35" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="I35" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="J35" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="K35" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="2">
+        <v>34</v>
+      </c>
       <c r="C36" s="14"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="14"/>
-      <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="14"/>
-      <c r="I36" s="14"/>
-      <c r="J36" s="14"/>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B37" s="14"/>
+      <c r="D36" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="G36" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="H36" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="I36" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="J36" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="K36" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B37" s="2">
+        <v>35</v>
+      </c>
       <c r="C37" s="14"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="14"/>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B38" s="14"/>
+      <c r="D37" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
+      <c r="H37" s="13"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B38" s="2">
+        <v>36</v>
+      </c>
       <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="14"/>
-      <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B39" s="14"/>
+      <c r="D38" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+      <c r="G38" s="13"/>
+      <c r="H38" s="13"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="13"/>
+      <c r="K38" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B39" s="2">
+        <v>37</v>
+      </c>
       <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="14"/>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B40" s="14"/>
+      <c r="D39" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="13"/>
+      <c r="K39" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B40" s="2">
+        <v>38</v>
+      </c>
       <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="14"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
-      <c r="I40" s="14"/>
-      <c r="J40" s="14"/>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B41" s="14"/>
+      <c r="D40" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="13"/>
+      <c r="K40" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B41" s="2">
+        <v>39</v>
+      </c>
       <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="14"/>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B42" s="14"/>
+      <c r="D41" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+      <c r="G41" s="13"/>
+      <c r="H41" s="13"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B42" s="2">
+        <v>40</v>
+      </c>
       <c r="C42" s="14"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="14"/>
-      <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="14"/>
-      <c r="I42" s="14"/>
-      <c r="J42" s="14"/>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B43" s="14"/>
+      <c r="D42" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+      <c r="G42" s="13"/>
+      <c r="H42" s="13"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="13"/>
+      <c r="K42" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B43" s="2">
+        <v>41</v>
+      </c>
       <c r="C43" s="14"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="14"/>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14"/>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B44" s="14"/>
+      <c r="D43" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13"/>
+      <c r="H43" s="13"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="13"/>
+      <c r="K43" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B44" s="2">
+        <v>42</v>
+      </c>
       <c r="C44" s="14"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="14"/>
-      <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="14"/>
-      <c r="I44" s="14"/>
-      <c r="J44" s="14"/>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B45" s="14"/>
+      <c r="D44" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="13"/>
+      <c r="J44" s="13"/>
+      <c r="K44" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B45" s="2">
+        <v>43</v>
+      </c>
       <c r="C45" s="14"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="14"/>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="14"/>
-      <c r="J45" s="14"/>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B46" s="14"/>
+      <c r="D45" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="13"/>
+      <c r="K45" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B46" s="2">
+        <v>44</v>
+      </c>
       <c r="C46" s="14"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="14"/>
-      <c r="F46" s="14"/>
-      <c r="G46" s="14"/>
-      <c r="H46" s="14"/>
-      <c r="I46" s="14"/>
-      <c r="J46" s="14"/>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B47" s="14"/>
+      <c r="D46" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="13"/>
+      <c r="K46" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B47" s="2">
+        <v>45</v>
+      </c>
       <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="14"/>
-      <c r="J47" s="14"/>
-    </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B48" s="14"/>
+      <c r="D47" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+      <c r="G47" s="13"/>
+      <c r="H47" s="13"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="13"/>
+      <c r="K47" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B48" s="2">
+        <v>46</v>
+      </c>
       <c r="C48" s="14"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="14"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="14"/>
-      <c r="J48" s="14"/>
-    </row>
-    <row r="49" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B49" s="14"/>
+      <c r="D48" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+      <c r="G48" s="13"/>
+      <c r="H48" s="13"/>
+      <c r="I48" s="13"/>
+      <c r="J48" s="13"/>
+      <c r="K48" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B49" s="2">
+        <v>47</v>
+      </c>
       <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="14"/>
-      <c r="J49" s="14"/>
-    </row>
-    <row r="50" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B50" s="14"/>
+      <c r="D49" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
+      <c r="I49" s="13"/>
+      <c r="J49" s="13"/>
+      <c r="K49" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B50" s="2">
+        <v>48</v>
+      </c>
       <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
-      <c r="I50" s="14"/>
-      <c r="J50" s="14"/>
-    </row>
-    <row r="51" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B51" s="14"/>
+      <c r="D50" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="13"/>
+      <c r="J50" s="13"/>
+      <c r="K50" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B51" s="2">
+        <v>49</v>
+      </c>
       <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
-      <c r="H51" s="14"/>
-      <c r="I51" s="14"/>
-      <c r="J51" s="14"/>
-    </row>
-    <row r="52" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B52" s="14"/>
+      <c r="D51" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13"/>
+      <c r="G51" s="13"/>
+      <c r="H51" s="13"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="13"/>
+      <c r="K51" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B52" s="2">
+        <v>50</v>
+      </c>
       <c r="C52" s="14"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="14"/>
-      <c r="J52" s="14"/>
-    </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B53" s="14"/>
+      <c r="D52" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E52" s="13"/>
+      <c r="F52" s="13"/>
+      <c r="G52" s="13"/>
+      <c r="H52" s="13"/>
+      <c r="I52" s="13"/>
+      <c r="J52" s="13"/>
+      <c r="K52" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B53" s="2">
+        <v>51</v>
+      </c>
       <c r="C53" s="14"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="14"/>
-      <c r="I53" s="14"/>
-      <c r="J53" s="14"/>
-    </row>
-    <row r="54" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B54" s="14"/>
+      <c r="D53" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13"/>
+      <c r="G53" s="13"/>
+      <c r="H53" s="13"/>
+      <c r="I53" s="13"/>
+      <c r="J53" s="13"/>
+      <c r="K53" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B54" s="2">
+        <v>52</v>
+      </c>
       <c r="C54" s="14"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
-      <c r="H54" s="14"/>
-      <c r="I54" s="14"/>
-      <c r="J54" s="14"/>
-    </row>
-    <row r="55" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B55" s="14"/>
+      <c r="D54" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E54" s="13"/>
+      <c r="F54" s="13"/>
+      <c r="G54" s="13"/>
+      <c r="H54" s="13"/>
+      <c r="I54" s="13"/>
+      <c r="J54" s="13"/>
+      <c r="K54" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B55" s="2">
+        <v>53</v>
+      </c>
       <c r="C55" s="14"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="14"/>
-      <c r="I55" s="14"/>
-      <c r="J55" s="14"/>
-    </row>
-    <row r="56" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B56" s="14"/>
+      <c r="D55" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E55" s="13"/>
+      <c r="F55" s="13"/>
+      <c r="G55" s="13"/>
+      <c r="H55" s="13"/>
+      <c r="I55" s="13"/>
+      <c r="J55" s="13"/>
+      <c r="K55" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B56" s="2">
+        <v>54</v>
+      </c>
       <c r="C56" s="14"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="14"/>
-      <c r="I56" s="14"/>
-      <c r="J56" s="14"/>
-    </row>
-    <row r="57" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B57" s="14"/>
+      <c r="D56" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
+      <c r="G56" s="13"/>
+      <c r="H56" s="13"/>
+      <c r="I56" s="13"/>
+      <c r="J56" s="13"/>
+      <c r="K56" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B57" s="2">
+        <v>55</v>
+      </c>
       <c r="C57" s="14"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
-      <c r="I57" s="14"/>
-      <c r="J57" s="14"/>
-    </row>
-    <row r="58" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B58" s="14"/>
+      <c r="D57" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="E57" s="13"/>
+      <c r="F57" s="13"/>
+      <c r="G57" s="13"/>
+      <c r="H57" s="13"/>
+      <c r="I57" s="13"/>
+      <c r="J57" s="13"/>
+      <c r="K57" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B58" s="2">
+        <v>56</v>
+      </c>
       <c r="C58" s="14"/>
-      <c r="D58" s="14"/>
-      <c r="E58" s="14"/>
-      <c r="F58" s="14"/>
-      <c r="G58" s="14"/>
-      <c r="H58" s="14"/>
-      <c r="I58" s="14"/>
-      <c r="J58" s="14"/>
-    </row>
-    <row r="59" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B59" s="14"/>
+      <c r="D58" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E58" s="13"/>
+      <c r="F58" s="13"/>
+      <c r="G58" s="13"/>
+      <c r="H58" s="13"/>
+      <c r="I58" s="13"/>
+      <c r="J58" s="13"/>
+      <c r="K58" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B59" s="2">
+        <v>57</v>
+      </c>
       <c r="C59" s="14"/>
-      <c r="D59" s="14"/>
-      <c r="E59" s="14"/>
-      <c r="F59" s="14"/>
-      <c r="G59" s="14"/>
-      <c r="H59" s="14"/>
-      <c r="I59" s="14"/>
-      <c r="J59" s="14"/>
-    </row>
-    <row r="60" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B60" s="14"/>
+      <c r="D59" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E59" s="13"/>
+      <c r="F59" s="13"/>
+      <c r="G59" s="13"/>
+      <c r="H59" s="13"/>
+      <c r="I59" s="13"/>
+      <c r="J59" s="13"/>
+      <c r="K59" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B60" s="2">
+        <v>58</v>
+      </c>
       <c r="C60" s="14"/>
-      <c r="D60" s="14"/>
-      <c r="E60" s="14"/>
-      <c r="F60" s="14"/>
-      <c r="G60" s="14"/>
-      <c r="H60" s="14"/>
-      <c r="I60" s="14"/>
-      <c r="J60" s="14"/>
-    </row>
-    <row r="61" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B61" s="14"/>
+      <c r="D60" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E60" s="13"/>
+      <c r="F60" s="13"/>
+      <c r="G60" s="13"/>
+      <c r="H60" s="13"/>
+      <c r="I60" s="13"/>
+      <c r="J60" s="13"/>
+      <c r="K60" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B61" s="2">
+        <v>59</v>
+      </c>
       <c r="C61" s="14"/>
-      <c r="D61" s="14"/>
-      <c r="E61" s="14"/>
-      <c r="F61" s="14"/>
-      <c r="G61" s="14"/>
-      <c r="H61" s="14"/>
-      <c r="I61" s="14"/>
-      <c r="J61" s="14"/>
-    </row>
-    <row r="62" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B62" s="14"/>
+      <c r="D61" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E61" s="13"/>
+      <c r="F61" s="13"/>
+      <c r="G61" s="13"/>
+      <c r="H61" s="13"/>
+      <c r="I61" s="13"/>
+      <c r="J61" s="13"/>
+      <c r="K61" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B62" s="2">
+        <v>60</v>
+      </c>
       <c r="C62" s="14"/>
-      <c r="D62" s="14"/>
-      <c r="E62" s="14"/>
-      <c r="F62" s="14"/>
-      <c r="G62" s="14"/>
-      <c r="H62" s="14"/>
-      <c r="I62" s="14"/>
-      <c r="J62" s="14"/>
-    </row>
-    <row r="63" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B63" s="14"/>
+      <c r="D62" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E62" s="13"/>
+      <c r="F62" s="13"/>
+      <c r="G62" s="13"/>
+      <c r="H62" s="13"/>
+      <c r="I62" s="13"/>
+      <c r="J62" s="13"/>
+      <c r="K62" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B63" s="2">
+        <v>61</v>
+      </c>
       <c r="C63" s="14"/>
-      <c r="D63" s="14"/>
-      <c r="E63" s="14"/>
-      <c r="F63" s="14"/>
-      <c r="G63" s="14"/>
-      <c r="H63" s="14"/>
-      <c r="I63" s="14"/>
-      <c r="J63" s="14"/>
-    </row>
-    <row r="64" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B64" s="14"/>
+      <c r="D63" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E63" s="13"/>
+      <c r="F63" s="13"/>
+      <c r="G63" s="13"/>
+      <c r="H63" s="13"/>
+      <c r="I63" s="13"/>
+      <c r="J63" s="13"/>
+      <c r="K63" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B64" s="2">
+        <v>62</v>
+      </c>
       <c r="C64" s="14"/>
-      <c r="D64" s="14"/>
-      <c r="E64" s="14"/>
-      <c r="F64" s="14"/>
-      <c r="G64" s="14"/>
-      <c r="H64" s="14"/>
-      <c r="I64" s="14"/>
-      <c r="J64" s="14"/>
-    </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B65" s="14"/>
+      <c r="D64" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E64" s="13"/>
+      <c r="F64" s="13"/>
+      <c r="G64" s="13"/>
+      <c r="H64" s="13"/>
+      <c r="I64" s="13"/>
+      <c r="J64" s="13"/>
+      <c r="K64" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B65" s="2">
+        <v>63</v>
+      </c>
       <c r="C65" s="14"/>
-      <c r="D65" s="14"/>
-      <c r="E65" s="14"/>
-      <c r="F65" s="14"/>
-      <c r="G65" s="14"/>
-      <c r="H65" s="14"/>
-      <c r="I65" s="14"/>
-      <c r="J65" s="14"/>
-    </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B66" s="14"/>
+      <c r="D65" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E65" s="13"/>
+      <c r="F65" s="13"/>
+      <c r="G65" s="13"/>
+      <c r="H65" s="13"/>
+      <c r="I65" s="13"/>
+      <c r="J65" s="13"/>
+      <c r="K65" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B66" s="2">
+        <v>64</v>
+      </c>
       <c r="C66" s="14"/>
-      <c r="D66" s="14"/>
-      <c r="E66" s="14"/>
-      <c r="F66" s="14"/>
-      <c r="G66" s="14"/>
-      <c r="H66" s="14"/>
-      <c r="I66" s="14"/>
-      <c r="J66" s="14"/>
-    </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B67" s="14"/>
+      <c r="D66" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="E66" s="13"/>
+      <c r="F66" s="13"/>
+      <c r="G66" s="13"/>
+      <c r="H66" s="13"/>
+      <c r="I66" s="13"/>
+      <c r="J66" s="13"/>
+      <c r="K66" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B67" s="2">
+        <v>65</v>
+      </c>
       <c r="C67" s="14"/>
-      <c r="D67" s="14"/>
-      <c r="E67" s="14"/>
-      <c r="F67" s="14"/>
-      <c r="G67" s="14"/>
-      <c r="H67" s="14"/>
-      <c r="I67" s="14"/>
-      <c r="J67" s="14"/>
-    </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B68" s="14"/>
+      <c r="D67" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E67" s="13"/>
+      <c r="F67" s="13"/>
+      <c r="G67" s="13"/>
+      <c r="H67" s="13"/>
+      <c r="I67" s="13"/>
+      <c r="J67" s="13"/>
+      <c r="K67" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B68" s="2">
+        <v>66</v>
+      </c>
       <c r="C68" s="14"/>
-      <c r="D68" s="14"/>
-      <c r="E68" s="14"/>
-      <c r="F68" s="14"/>
-      <c r="G68" s="14"/>
-      <c r="H68" s="14"/>
-      <c r="I68" s="14"/>
-      <c r="J68" s="14"/>
-    </row>
-    <row r="69" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B69" s="14"/>
+      <c r="D68" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="E68" s="13"/>
+      <c r="F68" s="13"/>
+      <c r="G68" s="13"/>
+      <c r="H68" s="13"/>
+      <c r="I68" s="13"/>
+      <c r="J68" s="13"/>
+      <c r="K68" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B69" s="2">
+        <v>67</v>
+      </c>
       <c r="C69" s="14"/>
-      <c r="D69" s="14"/>
-      <c r="E69" s="14"/>
-      <c r="F69" s="14"/>
-      <c r="G69" s="14"/>
-      <c r="H69" s="14"/>
-      <c r="I69" s="14"/>
-      <c r="J69" s="14"/>
-    </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B70" s="14"/>
+      <c r="D69" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E69" s="13"/>
+      <c r="F69" s="13"/>
+      <c r="G69" s="13"/>
+      <c r="H69" s="13"/>
+      <c r="I69" s="13"/>
+      <c r="J69" s="13"/>
+      <c r="K69" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B70" s="2">
+        <v>68</v>
+      </c>
       <c r="C70" s="14"/>
-      <c r="D70" s="14"/>
-      <c r="E70" s="14"/>
-      <c r="F70" s="14"/>
-      <c r="G70" s="14"/>
-      <c r="H70" s="14"/>
-      <c r="I70" s="14"/>
-      <c r="J70" s="14"/>
-    </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B71" s="14"/>
+      <c r="D70" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="E70" s="13"/>
+      <c r="F70" s="13"/>
+      <c r="G70" s="13"/>
+      <c r="H70" s="13"/>
+      <c r="I70" s="13"/>
+      <c r="J70" s="13"/>
+      <c r="K70" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B71" s="2">
+        <v>69</v>
+      </c>
       <c r="C71" s="14"/>
-      <c r="D71" s="14"/>
-      <c r="E71" s="14"/>
-      <c r="F71" s="14"/>
-      <c r="G71" s="14"/>
-      <c r="H71" s="14"/>
-      <c r="I71" s="14"/>
-      <c r="J71" s="14"/>
+      <c r="D71" s="2"/>
+      <c r="E71" s="13"/>
+      <c r="F71" s="13"/>
+      <c r="G71" s="13"/>
+      <c r="H71" s="13"/>
+      <c r="I71" s="13"/>
+      <c r="J71" s="13"/>
+      <c r="K71" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B72" s="2">
+        <v>70</v>
+      </c>
+      <c r="C72" s="14"/>
+      <c r="D72" s="2"/>
+      <c r="E72" s="13"/>
+      <c r="F72" s="13"/>
+      <c r="G72" s="13"/>
+      <c r="H72" s="13"/>
+      <c r="I72" s="13"/>
+      <c r="J72" s="13"/>
+      <c r="K72" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B73" s="2"/>
+      <c r="C73" s="14"/>
+      <c r="D73" s="2"/>
+      <c r="E73" s="13"/>
+      <c r="F73" s="13"/>
+      <c r="G73" s="13"/>
+      <c r="H73" s="13"/>
+      <c r="I73" s="13"/>
+      <c r="J73" s="13"/>
+      <c r="K73" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B74" s="2"/>
+      <c r="C74" s="14"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="13"/>
+      <c r="F74" s="13"/>
+      <c r="G74" s="13"/>
+      <c r="H74" s="13"/>
+      <c r="I74" s="13"/>
+      <c r="J74" s="13"/>
+      <c r="K74" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B75" s="2"/>
+      <c r="C75" s="14"/>
+      <c r="D75" s="2"/>
+      <c r="E75" s="13"/>
+      <c r="F75" s="13"/>
+      <c r="G75" s="13"/>
+      <c r="H75" s="13"/>
+      <c r="I75" s="13"/>
+      <c r="J75" s="13"/>
+      <c r="K75" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B76" s="2"/>
+      <c r="C76" s="14"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="13"/>
+      <c r="F76" s="13"/>
+      <c r="G76" s="13"/>
+      <c r="H76" s="13"/>
+      <c r="I76" s="13"/>
+      <c r="J76" s="13"/>
+      <c r="K76" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B77" s="2"/>
+      <c r="C77" s="14"/>
+      <c r="D77" s="2"/>
+      <c r="E77" s="13"/>
+      <c r="F77" s="13"/>
+      <c r="G77" s="13"/>
+      <c r="H77" s="13"/>
+      <c r="I77" s="13"/>
+      <c r="J77" s="13"/>
+      <c r="K77" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B78" s="2"/>
+      <c r="C78" s="14"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="13"/>
+      <c r="F78" s="13"/>
+      <c r="G78" s="13"/>
+      <c r="H78" s="13"/>
+      <c r="I78" s="13"/>
+      <c r="J78" s="13"/>
+      <c r="K78" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B79" s="2"/>
+      <c r="C79" s="14"/>
+      <c r="D79" s="2"/>
+      <c r="E79" s="13"/>
+      <c r="F79" s="13"/>
+      <c r="G79" s="13"/>
+      <c r="H79" s="13"/>
+      <c r="I79" s="13"/>
+      <c r="J79" s="13"/>
+      <c r="K79" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B80" s="2"/>
+      <c r="C80" s="14"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="13"/>
+      <c r="F80" s="13"/>
+      <c r="G80" s="13"/>
+      <c r="H80" s="13"/>
+      <c r="I80" s="13"/>
+      <c r="J80" s="13"/>
+      <c r="K80" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B81" s="2"/>
+      <c r="C81" s="14"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="13"/>
+      <c r="F81" s="13"/>
+      <c r="G81" s="13"/>
+      <c r="H81" s="13"/>
+      <c r="I81" s="13"/>
+      <c r="J81" s="13"/>
+      <c r="K81" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B82" s="2"/>
+      <c r="C82" s="14"/>
+      <c r="D82" s="2"/>
+      <c r="E82" s="13"/>
+      <c r="F82" s="13"/>
+      <c r="G82" s="13"/>
+      <c r="H82" s="13"/>
+      <c r="I82" s="13"/>
+      <c r="J82" s="13"/>
+      <c r="K82" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B83" s="2"/>
+      <c r="C83" s="14"/>
+      <c r="D83" s="2"/>
+      <c r="E83" s="13"/>
+      <c r="F83" s="13"/>
+      <c r="G83" s="13"/>
+      <c r="H83" s="13"/>
+      <c r="I83" s="13"/>
+      <c r="J83" s="13"/>
+      <c r="K83" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B84" s="2"/>
+      <c r="C84" s="14"/>
+      <c r="D84" s="2"/>
+      <c r="E84" s="13"/>
+      <c r="F84" s="13"/>
+      <c r="G84" s="13"/>
+      <c r="H84" s="13"/>
+      <c r="I84" s="13"/>
+      <c r="J84" s="13"/>
+      <c r="K84" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B85" s="2"/>
+      <c r="C85" s="14"/>
+      <c r="D85" s="2"/>
+      <c r="E85" s="13"/>
+      <c r="F85" s="13"/>
+      <c r="G85" s="13"/>
+      <c r="H85" s="13"/>
+      <c r="I85" s="13"/>
+      <c r="J85" s="13"/>
+      <c r="K85" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B86" s="2"/>
+      <c r="C86" s="14"/>
+      <c r="D86" s="2"/>
+      <c r="E86" s="13"/>
+      <c r="F86" s="13"/>
+      <c r="G86" s="13"/>
+      <c r="H86" s="13"/>
+      <c r="I86" s="13"/>
+      <c r="J86" s="13"/>
+      <c r="K86" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B87" s="2"/>
+      <c r="C87" s="14"/>
+      <c r="D87" s="2"/>
+      <c r="E87" s="13"/>
+      <c r="F87" s="13"/>
+      <c r="G87" s="13"/>
+      <c r="H87" s="13"/>
+      <c r="I87" s="13"/>
+      <c r="J87" s="13"/>
+      <c r="K87" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B88" s="2"/>
+      <c r="C88" s="14"/>
+      <c r="D88" s="2"/>
+      <c r="E88" s="13"/>
+      <c r="F88" s="13"/>
+      <c r="G88" s="13"/>
+      <c r="H88" s="13"/>
+      <c r="I88" s="13"/>
+      <c r="J88" s="13"/>
+      <c r="K88" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B89" s="2"/>
+      <c r="C89" s="14"/>
+      <c r="D89" s="2"/>
+      <c r="E89" s="13"/>
+      <c r="F89" s="13"/>
+      <c r="G89" s="13"/>
+      <c r="H89" s="13"/>
+      <c r="I89" s="13"/>
+      <c r="J89" s="13"/>
+      <c r="K89" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B90" s="14"/>
+      <c r="C90" s="14"/>
+      <c r="D90" s="14"/>
+      <c r="E90" s="14"/>
+      <c r="F90" s="14"/>
+      <c r="G90" s="14"/>
+      <c r="H90" s="14"/>
+      <c r="I90" s="14"/>
+      <c r="J90" s="14"/>
+    </row>
+    <row r="91" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B91" s="14"/>
+      <c r="C91" s="14"/>
+      <c r="D91" s="14"/>
+      <c r="E91" s="14"/>
+      <c r="F91" s="14"/>
+      <c r="G91" s="14"/>
+      <c r="H91" s="14"/>
+      <c r="I91" s="14"/>
+      <c r="J91" s="14"/>
+    </row>
+    <row r="92" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B92" s="14"/>
+      <c r="C92" s="14"/>
+      <c r="D92" s="14"/>
+      <c r="E92" s="14"/>
+      <c r="F92" s="14"/>
+      <c r="G92" s="14"/>
+      <c r="H92" s="14"/>
+      <c r="I92" s="14"/>
+      <c r="J92" s="14"/>
+    </row>
+    <row r="93" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B93" s="14"/>
+      <c r="C93" s="14"/>
+      <c r="D93" s="14"/>
+      <c r="E93" s="14"/>
+      <c r="F93" s="14"/>
+      <c r="G93" s="14"/>
+      <c r="H93" s="14"/>
+      <c r="I93" s="14"/>
+      <c r="J93" s="14"/>
+    </row>
+    <row r="94" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B94" s="14"/>
+      <c r="C94" s="14"/>
+      <c r="D94" s="14"/>
+      <c r="E94" s="14"/>
+      <c r="F94" s="14"/>
+      <c r="G94" s="14"/>
+      <c r="H94" s="14"/>
+      <c r="I94" s="14"/>
+      <c r="J94" s="14"/>
+    </row>
+    <row r="95" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B95" s="14"/>
+      <c r="C95" s="14"/>
+      <c r="D95" s="14"/>
+      <c r="E95" s="14"/>
+      <c r="F95" s="14"/>
+      <c r="G95" s="14"/>
+      <c r="H95" s="14"/>
+      <c r="I95" s="14"/>
+      <c r="J95" s="14"/>
+    </row>
+    <row r="96" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B96" s="14"/>
+      <c r="C96" s="14"/>
+      <c r="D96" s="14"/>
+      <c r="E96" s="14"/>
+      <c r="F96" s="14"/>
+      <c r="G96" s="14"/>
+      <c r="H96" s="14"/>
+      <c r="I96" s="14"/>
+      <c r="J96" s="14"/>
+    </row>
+    <row r="97" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B97" s="14"/>
+      <c r="C97" s="14"/>
+      <c r="D97" s="14"/>
+      <c r="E97" s="14"/>
+      <c r="F97" s="14"/>
+      <c r="G97" s="14"/>
+      <c r="H97" s="14"/>
+      <c r="I97" s="14"/>
+      <c r="J97" s="14"/>
+    </row>
+    <row r="98" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B98" s="14"/>
+      <c r="C98" s="14"/>
+      <c r="D98" s="14"/>
+      <c r="E98" s="14"/>
+      <c r="F98" s="14"/>
+      <c r="G98" s="14"/>
+      <c r="H98" s="14"/>
+      <c r="I98" s="14"/>
+      <c r="J98" s="14"/>
+    </row>
+    <row r="99" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B99" s="14"/>
+      <c r="C99" s="14"/>
+      <c r="D99" s="14"/>
+      <c r="E99" s="14"/>
+      <c r="F99" s="14"/>
+      <c r="G99" s="14"/>
+      <c r="H99" s="14"/>
+      <c r="I99" s="14"/>
+      <c r="J99" s="14"/>
+    </row>
+    <row r="100" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B100" s="14"/>
+      <c r="C100" s="14"/>
+      <c r="D100" s="14"/>
+      <c r="E100" s="14"/>
+      <c r="F100" s="14"/>
+      <c r="G100" s="14"/>
+      <c r="H100" s="14"/>
+      <c r="I100" s="14"/>
+      <c r="J100" s="14"/>
+    </row>
+    <row r="101" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B101" s="14"/>
+      <c r="C101" s="14"/>
+      <c r="D101" s="14"/>
+      <c r="E101" s="14"/>
+      <c r="F101" s="14"/>
+      <c r="G101" s="14"/>
+      <c r="H101" s="14"/>
+      <c r="I101" s="14"/>
+      <c r="J101" s="14"/>
+    </row>
+    <row r="102" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B102" s="14"/>
+      <c r="C102" s="14"/>
+      <c r="D102" s="14"/>
+      <c r="E102" s="14"/>
+      <c r="F102" s="14"/>
+      <c r="G102" s="14"/>
+      <c r="H102" s="14"/>
+      <c r="I102" s="14"/>
+      <c r="J102" s="14"/>
+    </row>
+    <row r="103" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B103" s="14"/>
+      <c r="C103" s="14"/>
+      <c r="D103" s="14"/>
+      <c r="E103" s="14"/>
+      <c r="F103" s="14"/>
+      <c r="G103" s="14"/>
+      <c r="H103" s="14"/>
+      <c r="I103" s="14"/>
+      <c r="J103" s="14"/>
+    </row>
+    <row r="104" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B104" s="14"/>
+      <c r="C104" s="14"/>
+      <c r="D104" s="14"/>
+      <c r="E104" s="14"/>
+      <c r="F104" s="14"/>
+      <c r="G104" s="14"/>
+      <c r="H104" s="14"/>
+      <c r="I104" s="14"/>
+      <c r="J104" s="14"/>
+    </row>
+    <row r="105" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B105" s="14"/>
+      <c r="C105" s="14"/>
+      <c r="D105" s="14"/>
+      <c r="E105" s="14"/>
+      <c r="F105" s="14"/>
+      <c r="G105" s="14"/>
+      <c r="H105" s="14"/>
+      <c r="I105" s="14"/>
+      <c r="J105" s="14"/>
+    </row>
+    <row r="106" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B106" s="14"/>
+      <c r="C106" s="14"/>
+      <c r="D106" s="14"/>
+      <c r="E106" s="14"/>
+      <c r="F106" s="14"/>
+      <c r="G106" s="14"/>
+      <c r="H106" s="14"/>
+      <c r="I106" s="14"/>
+      <c r="J106" s="14"/>
+    </row>
+    <row r="107" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B107" s="14"/>
+      <c r="C107" s="14"/>
+      <c r="D107" s="14"/>
+      <c r="E107" s="14"/>
+      <c r="F107" s="14"/>
+      <c r="G107" s="14"/>
+      <c r="H107" s="14"/>
+      <c r="I107" s="14"/>
+      <c r="J107" s="14"/>
+    </row>
+    <row r="108" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B108" s="14"/>
+      <c r="C108" s="14"/>
+      <c r="D108" s="14"/>
+      <c r="E108" s="14"/>
+      <c r="F108" s="14"/>
+      <c r="G108" s="14"/>
+      <c r="H108" s="14"/>
+      <c r="I108" s="14"/>
+      <c r="J108" s="14"/>
+    </row>
+    <row r="109" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B109" s="14"/>
+      <c r="C109" s="14"/>
+      <c r="D109" s="14"/>
+      <c r="E109" s="14"/>
+      <c r="F109" s="14"/>
+      <c r="G109" s="14"/>
+      <c r="H109" s="14"/>
+      <c r="I109" s="14"/>
+      <c r="J109" s="14"/>
+    </row>
+    <row r="110" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B110" s="14"/>
+      <c r="C110" s="14"/>
+      <c r="D110" s="14"/>
+      <c r="E110" s="14"/>
+      <c r="F110" s="14"/>
+      <c r="G110" s="14"/>
+      <c r="H110" s="14"/>
+      <c r="I110" s="14"/>
+      <c r="J110" s="14"/>
+    </row>
+    <row r="111" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B111" s="14"/>
+      <c r="C111" s="14"/>
+      <c r="D111" s="14"/>
+      <c r="E111" s="14"/>
+      <c r="F111" s="14"/>
+      <c r="G111" s="14"/>
+      <c r="H111" s="14"/>
+      <c r="I111" s="14"/>
+      <c r="J111" s="14"/>
+    </row>
+    <row r="112" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B112" s="14"/>
+      <c r="C112" s="14"/>
+      <c r="D112" s="14"/>
+      <c r="E112" s="14"/>
+      <c r="F112" s="14"/>
+      <c r="G112" s="14"/>
+      <c r="H112" s="14"/>
+      <c r="I112" s="14"/>
+      <c r="J112" s="14"/>
+    </row>
+    <row r="113" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B113" s="14"/>
+      <c r="C113" s="14"/>
+      <c r="D113" s="14"/>
+      <c r="E113" s="14"/>
+      <c r="F113" s="14"/>
+      <c r="G113" s="14"/>
+      <c r="H113" s="14"/>
+      <c r="I113" s="14"/>
+      <c r="J113" s="14"/>
+    </row>
+    <row r="114" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B114" s="14"/>
+      <c r="C114" s="14"/>
+      <c r="D114" s="14"/>
+      <c r="E114" s="14"/>
+      <c r="F114" s="14"/>
+      <c r="G114" s="14"/>
+      <c r="H114" s="14"/>
+      <c r="I114" s="14"/>
+      <c r="J114" s="14"/>
+    </row>
+    <row r="115" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B115" s="14"/>
+      <c r="C115" s="14"/>
+      <c r="D115" s="14"/>
+      <c r="E115" s="14"/>
+      <c r="F115" s="14"/>
+      <c r="G115" s="14"/>
+      <c r="H115" s="14"/>
+      <c r="I115" s="14"/>
+      <c r="J115" s="14"/>
+    </row>
+    <row r="116" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B116" s="14"/>
+      <c r="C116" s="14"/>
+      <c r="D116" s="14"/>
+      <c r="E116" s="14"/>
+      <c r="F116" s="14"/>
+      <c r="G116" s="14"/>
+      <c r="H116" s="14"/>
+      <c r="I116" s="14"/>
+      <c r="J116" s="14"/>
+    </row>
+    <row r="117" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B117" s="14"/>
+      <c r="C117" s="14"/>
+      <c r="D117" s="14"/>
+      <c r="E117" s="14"/>
+      <c r="F117" s="14"/>
+      <c r="G117" s="14"/>
+      <c r="H117" s="14"/>
+      <c r="I117" s="14"/>
+      <c r="J117" s="14"/>
+    </row>
+    <row r="118" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B118" s="14"/>
+      <c r="C118" s="14"/>
+      <c r="D118" s="14"/>
+      <c r="E118" s="14"/>
+      <c r="F118" s="14"/>
+      <c r="G118" s="14"/>
+      <c r="H118" s="14"/>
+      <c r="I118" s="14"/>
+      <c r="J118" s="14"/>
+    </row>
+    <row r="119" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B119" s="14"/>
+      <c r="C119" s="14"/>
+      <c r="D119" s="14"/>
+      <c r="E119" s="14"/>
+      <c r="F119" s="14"/>
+      <c r="G119" s="14"/>
+      <c r="H119" s="14"/>
+      <c r="I119" s="14"/>
+      <c r="J119" s="14"/>
+    </row>
+    <row r="120" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B120" s="14"/>
+      <c r="C120" s="14"/>
+      <c r="D120" s="14"/>
+      <c r="E120" s="14"/>
+      <c r="F120" s="14"/>
+      <c r="G120" s="14"/>
+      <c r="H120" s="14"/>
+      <c r="I120" s="14"/>
+      <c r="J120" s="14"/>
+    </row>
+    <row r="121" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B121" s="14"/>
+      <c r="C121" s="14"/>
+      <c r="D121" s="14"/>
+      <c r="E121" s="14"/>
+      <c r="F121" s="14"/>
+      <c r="G121" s="14"/>
+      <c r="H121" s="14"/>
+      <c r="I121" s="14"/>
+      <c r="J121" s="14"/>
+    </row>
+    <row r="122" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B122" s="14"/>
+      <c r="C122" s="14"/>
+      <c r="D122" s="14"/>
+      <c r="E122" s="14"/>
+      <c r="F122" s="14"/>
+      <c r="G122" s="14"/>
+      <c r="H122" s="14"/>
+      <c r="I122" s="14"/>
+      <c r="J122" s="14"/>
+    </row>
+    <row r="123" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B123" s="14"/>
+      <c r="C123" s="14"/>
+      <c r="D123" s="14"/>
+      <c r="E123" s="14"/>
+      <c r="F123" s="14"/>
+      <c r="G123" s="14"/>
+      <c r="H123" s="14"/>
+      <c r="I123" s="14"/>
+      <c r="J123" s="14"/>
+    </row>
+    <row r="124" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B124" s="14"/>
+      <c r="C124" s="14"/>
+      <c r="D124" s="14"/>
+      <c r="E124" s="14"/>
+      <c r="F124" s="14"/>
+      <c r="G124" s="14"/>
+      <c r="H124" s="14"/>
+      <c r="I124" s="14"/>
+      <c r="J124" s="14"/>
+    </row>
+    <row r="125" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B125" s="14"/>
+      <c r="C125" s="14"/>
+      <c r="D125" s="14"/>
+      <c r="E125" s="14"/>
+      <c r="F125" s="14"/>
+      <c r="G125" s="14"/>
+      <c r="H125" s="14"/>
+      <c r="I125" s="14"/>
+      <c r="J125" s="14"/>
+    </row>
+    <row r="126" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B126" s="14"/>
+      <c r="C126" s="14"/>
+      <c r="D126" s="14"/>
+      <c r="E126" s="14"/>
+      <c r="F126" s="14"/>
+      <c r="G126" s="14"/>
+      <c r="H126" s="14"/>
+      <c r="I126" s="14"/>
+      <c r="J126" s="14"/>
+    </row>
+    <row r="127" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B127" s="14"/>
+      <c r="C127" s="14"/>
+      <c r="D127" s="14"/>
+      <c r="E127" s="14"/>
+      <c r="F127" s="14"/>
+      <c r="G127" s="14"/>
+      <c r="H127" s="14"/>
+      <c r="I127" s="14"/>
+      <c r="J127" s="14"/>
+    </row>
+    <row r="128" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B128" s="14"/>
+      <c r="C128" s="14"/>
+      <c r="D128" s="14"/>
+      <c r="E128" s="14"/>
+      <c r="F128" s="14"/>
+      <c r="G128" s="14"/>
+      <c r="H128" s="14"/>
+      <c r="I128" s="14"/>
+      <c r="J128" s="14"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="K3:K22">
+  <phoneticPr fontId="4" type="noConversion"/>
+  <conditionalFormatting sqref="K3:K89">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Not Tested"</formula>
     </cfRule>
@@ -2883,7 +4552,7 @@
           <x14:formula1>
             <xm:f>Enums!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>K3:K22</xm:sqref>
+          <xm:sqref>K3:K89</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2938,6 +4607,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E81D8C8DDAE8BD44A422697963F06C45" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b6816e004dbb89c674e51f5647972552">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2b02348f-b4e3-458c-83fc-9e90db0f8029" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e6418ca14ac9ee17b8bbf6df78e0c223" ns2:_="">
     <xsd:import namespace="2b02348f-b4e3-458c-83fc-9e90db0f8029"/>
@@ -3095,22 +4779,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69DB72C7-DF0B-4E18-8174-00AB852E6FB4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2b02348f-b4e3-458c-83fc-9e90db0f8029"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{859B513B-8BED-4B59-B224-E0A2C6173D25}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCDB6385-31B2-4574-9AA4-BF13B563A4E3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3126,28 +4819,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{859B513B-8BED-4B59-B224-E0A2C6173D25}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69DB72C7-DF0B-4E18-8174-00AB852E6FB4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2b02348f-b4e3-458c-83fc-9e90db0f8029"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added System test cases till req-36
</commit_message>
<xml_diff>
--- a/docs/System_Test_Report_template.xlsx
+++ b/docs/System_Test_Report_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEB041A-E3BB-44D2-AA2A-0D595A2EDE60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F608835-7C5D-45C5-9AD9-5655C72CE4CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="215">
   <si>
     <t>Total Test Cases</t>
   </si>
@@ -650,6 +650,39 @@
   </si>
   <si>
     <t>App must be installed and account is created</t>
+  </si>
+  <si>
+    <t>Test if If No match is found in REQ-31 App shall show a notification to user for wrong password</t>
+  </si>
+  <si>
+    <t>Open the app and input random characters into the adm and password fields</t>
+  </si>
+  <si>
+    <t xml:space="preserve">App shows a snackbar indicating wrong login details </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test that From req-33, user should be prompted by 2 buttons 1 to reserve book and 1 to view borrowed books </t>
+  </si>
+  <si>
+    <t>App must show 2 buttons in homepage</t>
+  </si>
+  <si>
+    <t>App must show 2 buttons in homepage one to reserve and 1 to view loaned books</t>
+  </si>
+  <si>
+    <t>Test that</t>
+  </si>
+  <si>
+    <t>Test that If user selects to view borrowed books, A list of reserved books and their loaned dates, title and location should be shown to user</t>
+  </si>
+  <si>
+    <t>App must be installed and account is created and logged in</t>
+  </si>
+  <si>
+    <t>presses the view the view loaned books button</t>
+  </si>
+  <si>
+    <t>App must show a list of boxes with the loaned/reserved book's date on loan, title and location</t>
   </si>
 </sst>
 </file>
@@ -2120,8 +2153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:K128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J36" sqref="J36"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3216,7 +3249,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B37" s="2">
         <v>35</v>
       </c>
@@ -3224,17 +3257,29 @@
       <c r="D37" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="13"/>
-      <c r="H37" s="13"/>
-      <c r="I37" s="13"/>
-      <c r="J37" s="13"/>
+      <c r="E37" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F37" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="G37" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="H37" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="I37" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="J37" s="13" t="s">
+        <v>206</v>
+      </c>
       <c r="K37" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B38" s="2">
         <v>36</v>
       </c>
@@ -3242,17 +3287,29 @@
       <c r="D38" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
-      <c r="J38" s="13"/>
+      <c r="E38" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F38" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="G38" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="H38" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="I38" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="J38" s="13" t="s">
+        <v>208</v>
+      </c>
       <c r="K38" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:11" ht="72" x14ac:dyDescent="0.3">
       <c r="B39" s="2">
         <v>37</v>
       </c>
@@ -3260,12 +3317,24 @@
       <c r="D39" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="13"/>
-      <c r="H39" s="13"/>
-      <c r="I39" s="13"/>
-      <c r="J39" s="13"/>
+      <c r="E39" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="G39" s="13" t="s">
+        <v>212</v>
+      </c>
+      <c r="H39" s="13" t="s">
+        <v>213</v>
+      </c>
+      <c r="I39" s="13" t="s">
+        <v>214</v>
+      </c>
+      <c r="J39" s="13" t="s">
+        <v>214</v>
+      </c>
       <c r="K39" s="9" t="s">
         <v>3</v>
       </c>
@@ -3279,7 +3348,9 @@
         <v>160</v>
       </c>
       <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
+      <c r="F40" s="13" t="s">
+        <v>210</v>
+      </c>
       <c r="G40" s="13"/>
       <c r="H40" s="13"/>
       <c r="I40" s="13"/>
@@ -4607,21 +4678,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E81D8C8DDAE8BD44A422697963F06C45" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b6816e004dbb89c674e51f5647972552">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2b02348f-b4e3-458c-83fc-9e90db0f8029" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e6418ca14ac9ee17b8bbf6df78e0c223" ns2:_="">
     <xsd:import namespace="2b02348f-b4e3-458c-83fc-9e90db0f8029"/>
@@ -4779,31 +4835,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69DB72C7-DF0B-4E18-8174-00AB852E6FB4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2b02348f-b4e3-458c-83fc-9e90db0f8029"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{859B513B-8BED-4B59-B224-E0A2C6173D25}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCDB6385-31B2-4574-9AA4-BF13B563A4E3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4819,4 +4866,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{859B513B-8BED-4B59-B224-E0A2C6173D25}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69DB72C7-DF0B-4E18-8174-00AB852E6FB4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2b02348f-b4e3-458c-83fc-9e90db0f8029"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added system test case for Req-37 & 38
</commit_message>
<xml_diff>
--- a/docs/System_Test_Report_template.xlsx
+++ b/docs/System_Test_Report_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F608835-7C5D-45C5-9AD9-5655C72CE4CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E47B6524-295E-45AD-AC63-CB48DF629262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="223">
   <si>
     <t>Total Test Cases</t>
   </si>
@@ -670,9 +670,6 @@
     <t>App must show 2 buttons in homepage one to reserve and 1 to view loaned books</t>
   </si>
   <si>
-    <t>Test that</t>
-  </si>
-  <si>
     <t>Test that If user selects to view borrowed books, A list of reserved books and their loaned dates, title and location should be shown to user</t>
   </si>
   <si>
@@ -683,6 +680,33 @@
   </si>
   <si>
     <t>App must show a list of boxes with the loaned/reserved book's date on loan, title and location</t>
+  </si>
+  <si>
+    <t>Test that If user chooses to reserve book, a map of Singapore with all available libraries shows up.</t>
+  </si>
+  <si>
+    <t>App is logged in and user allowed location permissions to app</t>
+  </si>
+  <si>
+    <t>presses the view the reserve books button</t>
+  </si>
+  <si>
+    <t>A map of Singapore with 2 locations (1 at semb and 1 at woodlands show up)</t>
+  </si>
+  <si>
+    <t>Test that Once user picks a location, App shall display a list of book titles not already reserved or borrowed and is available at that location</t>
+  </si>
+  <si>
+    <t>User selects a location in map</t>
+  </si>
+  <si>
+    <t>Pick woodlands on the map</t>
+  </si>
+  <si>
+    <t>A list of books located at woodlands library shows up (that is not reserved or loaned) look out for pytest_book</t>
+  </si>
+  <si>
+    <t>a list of books is shown all of which is not loaned and reserved and at woodlands</t>
   </si>
 </sst>
 </file>
@@ -2153,8 +2177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:K128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3321,25 +3345,25 @@
         <v>13</v>
       </c>
       <c r="F39" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="G39" s="13" t="s">
         <v>211</v>
       </c>
-      <c r="G39" s="13" t="s">
+      <c r="H39" s="13" t="s">
         <v>212</v>
       </c>
-      <c r="H39" s="13" t="s">
+      <c r="I39" s="13" t="s">
         <v>213</v>
       </c>
-      <c r="I39" s="13" t="s">
-        <v>214</v>
-      </c>
       <c r="J39" s="13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K39" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B40" s="2">
         <v>38</v>
       </c>
@@ -3347,19 +3371,29 @@
       <c r="D40" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="E40" s="13"/>
+      <c r="E40" s="13" t="s">
+        <v>16</v>
+      </c>
       <c r="F40" s="13" t="s">
-        <v>210</v>
-      </c>
-      <c r="G40" s="13"/>
-      <c r="H40" s="13"/>
-      <c r="I40" s="13"/>
-      <c r="J40" s="13"/>
+        <v>214</v>
+      </c>
+      <c r="G40" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="H40" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="I40" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="J40" s="13" t="s">
+        <v>217</v>
+      </c>
       <c r="K40" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B41" s="2">
         <v>39</v>
       </c>
@@ -3367,12 +3401,24 @@
       <c r="D41" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="13"/>
-      <c r="I41" s="13"/>
-      <c r="J41" s="13"/>
+      <c r="E41" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="G41" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="H41" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="I41" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="J41" s="13" t="s">
+        <v>222</v>
+      </c>
       <c r="K41" s="9" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Added System test cases REQ39-41
</commit_message>
<xml_diff>
--- a/docs/System_Test_Report_template.xlsx
+++ b/docs/System_Test_Report_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E47B6524-295E-45AD-AC63-CB48DF629262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA52FC71-9086-4A5D-A286-F9844921ECED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="235">
   <si>
     <t>Total Test Cases</t>
   </si>
@@ -707,6 +707,43 @@
   </si>
   <si>
     <t>a list of books is shown all of which is not loaned and reserved and at woodlands</t>
+  </si>
+  <si>
+    <t>test that App have a search bar to search for books</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pick woodlands on the map
+A search bar at the top appears and the user can input any words and filter by title, input "py" </t>
+  </si>
+  <si>
+    <t>Books filteed should contain the prompt in the title like pytest_book</t>
+  </si>
+  <si>
+    <t>List only contain book with the prompt in the title like pytest_book</t>
+  </si>
+  <si>
+    <t>Test that If user picks a book, they shall be prompted to confirm the borrow, or find out more using AI</t>
+  </si>
+  <si>
+    <t>User must pick a book from woodlands library</t>
+  </si>
+  <si>
+    <t>3 buttons should come up labelled AI, Borrow or cancel</t>
+  </si>
+  <si>
+    <t>3 buttons comes up labelled AI, Borrow or cancel</t>
+  </si>
+  <si>
+    <t>Pick any book from the list of available book In woodlands and press its item</t>
+  </si>
+  <si>
+    <t>Test that If AI is chosen, The app should send a prompt to Claude API asking for more details about the book chosenc</t>
+  </si>
+  <si>
+    <t>Pick any book from the list of available book In woodlands and press its item then select AI</t>
+  </si>
+  <si>
+    <t>Claude API activity tracker show increase in incoming tokens</t>
   </si>
 </sst>
 </file>
@@ -2177,8 +2214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:K128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H44" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3393,7 +3430,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="2:11" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:11" ht="87" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B41" s="2">
         <v>39</v>
       </c>
@@ -3423,7 +3460,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:11" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B42" s="2">
         <v>40</v>
       </c>
@@ -3431,17 +3468,29 @@
       <c r="D42" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="13"/>
-      <c r="I42" s="13"/>
-      <c r="J42" s="13"/>
+      <c r="E42" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F42" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="G42" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="H42" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="I42" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="J42" s="13" t="s">
+        <v>226</v>
+      </c>
       <c r="K42" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B43" s="2">
         <v>41</v>
       </c>
@@ -3449,17 +3498,29 @@
       <c r="D43" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="13"/>
-      <c r="I43" s="13"/>
-      <c r="J43" s="13"/>
+      <c r="E43" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F43" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="G43" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="H43" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="I43" s="13" t="s">
+        <v>229</v>
+      </c>
+      <c r="J43" s="13" t="s">
+        <v>230</v>
+      </c>
       <c r="K43" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B44" s="2">
         <v>42</v>
       </c>
@@ -3467,12 +3528,24 @@
       <c r="D44" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
-      <c r="H44" s="13"/>
-      <c r="I44" s="13"/>
-      <c r="J44" s="13"/>
+      <c r="E44" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F44" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="G44" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="H44" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="I44" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="J44" s="13" t="s">
+        <v>234</v>
+      </c>
       <c r="K44" s="9" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Added System test cases REQ42-44
</commit_message>
<xml_diff>
--- a/docs/System_Test_Report_template.xlsx
+++ b/docs/System_Test_Report_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA52FC71-9086-4A5D-A286-F9844921ECED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8434E972-4393-43C1-A066-FA20D69057CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="245">
   <si>
     <t>Total Test Cases</t>
   </si>
@@ -744,6 +744,36 @@
   </si>
   <si>
     <t>Claude API activity tracker show increase in incoming tokens</t>
+  </si>
+  <si>
+    <t>Test that The app waits for the response and display the description</t>
+  </si>
+  <si>
+    <t>A description of the Book should be shown on the page</t>
+  </si>
+  <si>
+    <t>A description of the Book shown on the page</t>
+  </si>
+  <si>
+    <t>Test that Once user confirms, App should check if the user has borrowed 10 books already</t>
+  </si>
+  <si>
+    <t>Pick any book from the list of available book In woodlands and press its item then select Borrow</t>
+  </si>
+  <si>
+    <t>No visible output, go to next test case</t>
+  </si>
+  <si>
+    <t>If the user has borrowed more than 10 books from REQ-43, the app should reject the reservation</t>
+  </si>
+  <si>
+    <t>User must pick a book from woodlands library and borrow it</t>
+  </si>
+  <si>
+    <t>Borrow 10 books through the previous steps then try to borrow an 11th one</t>
+  </si>
+  <si>
+    <t>Snackbar appears and disallow the reservation</t>
   </si>
 </sst>
 </file>
@@ -2214,8 +2244,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:K128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H44" sqref="H44"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3550,7 +3580,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B45" s="2">
         <v>43</v>
       </c>
@@ -3558,17 +3588,29 @@
       <c r="D45" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="13"/>
-      <c r="I45" s="13"/>
-      <c r="J45" s="13"/>
+      <c r="E45" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F45" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="G45" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="H45" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="I45" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="J45" s="13" t="s">
+        <v>237</v>
+      </c>
       <c r="K45" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B46" s="2">
         <v>44</v>
       </c>
@@ -3576,17 +3618,29 @@
       <c r="D46" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-      <c r="G46" s="13"/>
-      <c r="H46" s="13"/>
-      <c r="I46" s="13"/>
-      <c r="J46" s="13"/>
+      <c r="E46" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F46" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="G46" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="H46" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="I46" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="J46" s="13" t="s">
+        <v>240</v>
+      </c>
       <c r="K46" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B47" s="2">
         <v>45</v>
       </c>
@@ -3594,12 +3648,24 @@
       <c r="D47" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="13"/>
-      <c r="H47" s="13"/>
-      <c r="I47" s="13"/>
-      <c r="J47" s="13"/>
+      <c r="E47" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F47" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="G47" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="H47" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="I47" s="13" t="s">
+        <v>244</v>
+      </c>
+      <c r="J47" s="13" t="s">
+        <v>244</v>
+      </c>
       <c r="K47" s="9" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Added System test cases REQ45-46
</commit_message>
<xml_diff>
--- a/docs/System_Test_Report_template.xlsx
+++ b/docs/System_Test_Report_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8434E972-4393-43C1-A066-FA20D69057CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188347BF-A7D3-43F6-9452-EA517D46406D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="255">
   <si>
     <t>Total Test Cases</t>
   </si>
@@ -774,6 +774,36 @@
   </si>
   <si>
     <t>Snackbar appears and disallow the reservation</t>
+  </si>
+  <si>
+    <t>Test that If not flagged by REQ-44 App should update the books firebase entry with the user’s id, the date, and reservation status</t>
+  </si>
+  <si>
+    <t>User must pick a book from woodlands library and borrow it, there must be less then 10 books already loaned on the account</t>
+  </si>
+  <si>
+    <t>Select a book and try to reserve it</t>
+  </si>
+  <si>
+    <t>App allow the reservation and the book should now be listed on the list of books loaned by user</t>
+  </si>
+  <si>
+    <t>Test that From REQ-36 If a user taps on a book they have borrowed, the app should prompt the user if they want to extend the reservation</t>
+  </si>
+  <si>
+    <t>User must open their loaned list and click on a book on the list</t>
+  </si>
+  <si>
+    <t>Select a book in the list by pressing its box</t>
+  </si>
+  <si>
+    <t>Prompt asking user if they want to extend their reservation comes up</t>
+  </si>
+  <si>
+    <t>test that From REQ-46 If the user confirms, the app should check if the book has already been extended</t>
+  </si>
+  <si>
+    <t>test that If the book has already been extended the app should show an error message rejecting the extension</t>
   </si>
 </sst>
 </file>
@@ -2244,8 +2274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:K128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3670,7 +3700,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B48" s="2">
         <v>46</v>
       </c>
@@ -3678,17 +3708,29 @@
       <c r="D48" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="E48" s="13"/>
-      <c r="F48" s="13"/>
-      <c r="G48" s="13"/>
-      <c r="H48" s="13"/>
-      <c r="I48" s="13"/>
-      <c r="J48" s="13"/>
+      <c r="E48" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F48" s="13" t="s">
+        <v>245</v>
+      </c>
+      <c r="G48" s="13" t="s">
+        <v>246</v>
+      </c>
+      <c r="H48" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="I48" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="J48" s="13" t="s">
+        <v>248</v>
+      </c>
       <c r="K48" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:11" ht="72" x14ac:dyDescent="0.3">
       <c r="B49" s="2">
         <v>47</v>
       </c>
@@ -3696,17 +3738,29 @@
       <c r="D49" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
-      <c r="H49" s="13"/>
-      <c r="I49" s="13"/>
-      <c r="J49" s="13"/>
+      <c r="E49" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F49" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="G49" s="13" t="s">
+        <v>250</v>
+      </c>
+      <c r="H49" s="13" t="s">
+        <v>251</v>
+      </c>
+      <c r="I49" s="13" t="s">
+        <v>252</v>
+      </c>
+      <c r="J49" s="13" t="s">
+        <v>252</v>
+      </c>
       <c r="K49" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B50" s="2">
         <v>48</v>
       </c>
@@ -3715,7 +3769,9 @@
         <v>170</v>
       </c>
       <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
+      <c r="F50" s="13" t="s">
+        <v>253</v>
+      </c>
       <c r="G50" s="13"/>
       <c r="H50" s="13"/>
       <c r="I50" s="13"/>
@@ -3724,7 +3780,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B51" s="2">
         <v>49</v>
       </c>
@@ -3733,7 +3789,9 @@
         <v>171</v>
       </c>
       <c r="E51" s="13"/>
-      <c r="F51" s="13"/>
+      <c r="F51" s="13" t="s">
+        <v>254</v>
+      </c>
       <c r="G51" s="13"/>
       <c r="H51" s="13"/>
       <c r="I51" s="13"/>

</xml_diff>

<commit_message>
Added System test cases REQ47-48
</commit_message>
<xml_diff>
--- a/docs/System_Test_Report_template.xlsx
+++ b/docs/System_Test_Report_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{188347BF-A7D3-43F6-9452-EA517D46406D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B5BED4-BFA4-46A5-B6B7-F3D228793844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="260">
   <si>
     <t>Total Test Cases</t>
   </si>
@@ -804,6 +804,21 @@
   </si>
   <si>
     <t>test that If the book has already been extended the app should show an error message rejecting the extension</t>
+  </si>
+  <si>
+    <t>User must try to extend a reservation</t>
+  </si>
+  <si>
+    <t>Select a already loaned book and try to extend it</t>
+  </si>
+  <si>
+    <t>User must try to extend a loan that has already been extended</t>
+  </si>
+  <si>
+    <t>Select a already loaned book and extend it, then extend it again</t>
+  </si>
+  <si>
+    <t>Snackbar appears and disallow the extenstion</t>
   </si>
 </sst>
 </file>
@@ -2275,7 +2290,7 @@
   <dimension ref="B2:K128"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A48" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+      <selection activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3768,14 +3783,24 @@
       <c r="D50" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="E50" s="13"/>
+      <c r="E50" s="13" t="s">
+        <v>16</v>
+      </c>
       <c r="F50" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="G50" s="13"/>
-      <c r="H50" s="13"/>
-      <c r="I50" s="13"/>
-      <c r="J50" s="13"/>
+      <c r="G50" s="13" t="s">
+        <v>255</v>
+      </c>
+      <c r="H50" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="I50" s="13" t="s">
+        <v>240</v>
+      </c>
+      <c r="J50" s="13" t="s">
+        <v>240</v>
+      </c>
       <c r="K50" s="9" t="s">
         <v>3</v>
       </c>
@@ -3788,14 +3813,24 @@
       <c r="D51" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="E51" s="13"/>
+      <c r="E51" s="13" t="s">
+        <v>16</v>
+      </c>
       <c r="F51" s="13" t="s">
         <v>254</v>
       </c>
-      <c r="G51" s="13"/>
-      <c r="H51" s="13"/>
-      <c r="I51" s="13"/>
-      <c r="J51" s="13"/>
+      <c r="G51" s="13" t="s">
+        <v>257</v>
+      </c>
+      <c r="H51" s="13" t="s">
+        <v>258</v>
+      </c>
+      <c r="I51" s="13" t="s">
+        <v>259</v>
+      </c>
+      <c r="J51" s="13" t="s">
+        <v>259</v>
+      </c>
       <c r="K51" s="9" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Added System test cases REQ49-50
</commit_message>
<xml_diff>
--- a/docs/System_Test_Report_template.xlsx
+++ b/docs/System_Test_Report_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90B5BED4-BFA4-46A5-B6B7-F3D228793844}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B520CFA6-2213-4A11-AC7A-45E6814B6402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="268">
   <si>
     <t>Total Test Cases</t>
   </si>
@@ -819,6 +819,30 @@
   </si>
   <si>
     <t>Snackbar appears and disallow the extenstion</t>
+  </si>
+  <si>
+    <t>If the book has not already been extended the app should update the books firebase to indicated that it has been extended and move</t>
+  </si>
+  <si>
+    <t>User must try to extend a loan that has not already been extended</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select a already loaned book and extend it, </t>
+  </si>
+  <si>
+    <t>App redirects to main page and firebase book entry shows extended</t>
+  </si>
+  <si>
+    <t>Test that Every day at a set time clear non collected reservations</t>
+  </si>
+  <si>
+    <t>There has to be books that are over due and not collected</t>
+  </si>
+  <si>
+    <t>Use test account P2426082 to reserve a book, then change the date on firebase to more then 7 days ago, then run the RPI and wait 24 hours</t>
+  </si>
+  <si>
+    <t>The book reservation status will be cleared from the system and show up on the list of avaiable book in app</t>
   </si>
 </sst>
 </file>
@@ -2289,8 +2313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:K128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J51" sqref="J51"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3805,7 +3829,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:11" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B51" s="2">
         <v>49</v>
       </c>
@@ -3835,7 +3859,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:11" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B52" s="2">
         <v>50</v>
       </c>
@@ -3843,17 +3867,29 @@
       <c r="D52" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="E52" s="13"/>
-      <c r="F52" s="13"/>
-      <c r="G52" s="13"/>
-      <c r="H52" s="13"/>
-      <c r="I52" s="13"/>
-      <c r="J52" s="13"/>
+      <c r="E52" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F52" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="G52" s="13" t="s">
+        <v>261</v>
+      </c>
+      <c r="H52" s="13" t="s">
+        <v>262</v>
+      </c>
+      <c r="I52" s="13" t="s">
+        <v>263</v>
+      </c>
+      <c r="J52" s="13" t="s">
+        <v>263</v>
+      </c>
       <c r="K52" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B53" s="2">
         <v>51</v>
       </c>
@@ -3861,12 +3897,24 @@
       <c r="D53" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="E53" s="13"/>
-      <c r="F53" s="13"/>
-      <c r="G53" s="13"/>
-      <c r="H53" s="13"/>
-      <c r="I53" s="13"/>
-      <c r="J53" s="13"/>
+      <c r="E53" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F53" s="13" t="s">
+        <v>264</v>
+      </c>
+      <c r="G53" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="H53" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="I53" s="13" t="s">
+        <v>267</v>
+      </c>
+      <c r="J53" s="13" t="s">
+        <v>267</v>
+      </c>
       <c r="K53" s="9" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Added System test cases REQ51-53
</commit_message>
<xml_diff>
--- a/docs/System_Test_Report_template.xlsx
+++ b/docs/System_Test_Report_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B520CFA6-2213-4A11-AC7A-45E6814B6402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B741455D-73B4-4D1A-A61D-3B4D7393C9CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="277">
   <si>
     <t>Total Test Cases</t>
   </si>
@@ -843,6 +843,33 @@
   </si>
   <si>
     <t>The book reservation status will be cleared from the system and show up on the list of avaiable book in app</t>
+  </si>
+  <si>
+    <t>Test that A Website running on flask should be available for library staff to access</t>
+  </si>
+  <si>
+    <t>WebApp/app.py is ran seperately from main.py in Src</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On a browser while connecting to the same network as the RPI, type in the RPI's IP address:5000 </t>
+  </si>
+  <si>
+    <t>A mainpage website shows</t>
+  </si>
+  <si>
+    <t>Test that The website should have a search function for library staff to search a book by its title and see its details like onloan status, reserved status, borrower id, date of borrowing, bookid and location</t>
+  </si>
+  <si>
+    <t>On the mainmenu press the go to book search button, if a text is typed in the text field and the search button is pressed, the list of books will be narrowed to the books which contain the text in the title</t>
+  </si>
+  <si>
+    <t>A list of filtered books shows</t>
+  </si>
+  <si>
+    <t>Test that The Staff should also have the option to filter the list of books by location, reservation status and loan status</t>
+  </si>
+  <si>
+    <t>Same steps as REQ-52 but now with text fields for location, reservation status and loan status</t>
   </si>
 </sst>
 </file>
@@ -2313,8 +2340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:K128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I58" sqref="I58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3919,7 +3946,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B54" s="2">
         <v>52</v>
       </c>
@@ -3927,17 +3954,29 @@
       <c r="D54" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="E54" s="13"/>
-      <c r="F54" s="13"/>
-      <c r="G54" s="13"/>
-      <c r="H54" s="13"/>
-      <c r="I54" s="13"/>
-      <c r="J54" s="13"/>
+      <c r="E54" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F54" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="G54" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="H54" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="I54" s="13" t="s">
+        <v>271</v>
+      </c>
+      <c r="J54" s="13" t="s">
+        <v>271</v>
+      </c>
       <c r="K54" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="B55" s="2">
         <v>53</v>
       </c>
@@ -3945,17 +3984,29 @@
       <c r="D55" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="E55" s="13"/>
-      <c r="F55" s="13"/>
-      <c r="G55" s="13"/>
-      <c r="H55" s="13"/>
-      <c r="I55" s="13"/>
-      <c r="J55" s="13"/>
+      <c r="E55" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F55" s="13" t="s">
+        <v>272</v>
+      </c>
+      <c r="G55" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="H55" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="I55" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="J55" s="13" t="s">
+        <v>274</v>
+      </c>
       <c r="K55" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:11" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B56" s="2">
         <v>54</v>
       </c>
@@ -3963,12 +4014,24 @@
       <c r="D56" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="E56" s="13"/>
-      <c r="F56" s="13"/>
-      <c r="G56" s="13"/>
-      <c r="H56" s="13"/>
-      <c r="I56" s="13"/>
-      <c r="J56" s="13"/>
+      <c r="E56" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F56" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="G56" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="H56" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="I56" s="13" t="s">
+        <v>274</v>
+      </c>
+      <c r="J56" s="13" t="s">
+        <v>274</v>
+      </c>
       <c r="K56" s="9" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Added System test cases REQ54-56
</commit_message>
<xml_diff>
--- a/docs/System_Test_Report_template.xlsx
+++ b/docs/System_Test_Report_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B741455D-73B4-4D1A-A61D-3B4D7393C9CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E830FC-4CE7-4326-BC00-1CE66BC8138E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="289">
   <si>
     <t>Total Test Cases</t>
   </si>
@@ -870,6 +870,42 @@
   </si>
   <si>
     <t>Same steps as REQ-52 but now with text fields for location, reservation status and loan status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test that The Website should have a search function for library staff to search a user by their id number and display their fine amount and borrowed/loaned books </t>
+  </si>
+  <si>
+    <t>On the mainmenu press the go to user search button, if a text is typed in the text field and the search button is pressed, the list of users will be narrowed to the users which contain the text in the id</t>
+  </si>
+  <si>
+    <t>A list of filtered Users show</t>
+  </si>
+  <si>
+    <t>test that For both REQ 52 and 53, the staff must have a option to update all details of the user or book on the website.</t>
+  </si>
+  <si>
+    <t>Either user search or book search is clicked</t>
+  </si>
+  <si>
+    <t>At the bottom of every user/book there is an update button, click it and it will bring the staff to a page where she can enter the updated details and change it</t>
+  </si>
+  <si>
+    <t>User/Book detail is changed on firebase upon updating</t>
+  </si>
+  <si>
+    <t>Test that The staff should also have an option to reset a book’s reservation status thru a hotkey.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> book search is clicked</t>
+  </si>
+  <si>
+    <t>When in the edit page, a button can be pressed to quick set the book data to original state</t>
+  </si>
+  <si>
+    <t>Book will be shown in database to have no loanadm, reservation or loaned status or date</t>
+  </si>
+  <si>
+    <t>Book shown in database to have no loanadm, reservation or loaned status or date</t>
   </si>
 </sst>
 </file>
@@ -2340,7 +2376,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:K128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="I58" sqref="I58"/>
     </sheetView>
   </sheetViews>
@@ -4036,7 +4072,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:11" ht="115.2" x14ac:dyDescent="0.3">
       <c r="B57" s="2">
         <v>55</v>
       </c>
@@ -4044,17 +4080,29 @@
       <c r="D57" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="E57" s="13"/>
-      <c r="F57" s="13"/>
-      <c r="G57" s="13"/>
-      <c r="H57" s="13"/>
-      <c r="I57" s="13"/>
-      <c r="J57" s="13"/>
+      <c r="E57" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F57" s="13" t="s">
+        <v>277</v>
+      </c>
+      <c r="G57" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="H57" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="I57" s="13" t="s">
+        <v>279</v>
+      </c>
+      <c r="J57" s="13" t="s">
+        <v>279</v>
+      </c>
       <c r="K57" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B58" s="2">
         <v>56</v>
       </c>
@@ -4062,17 +4110,29 @@
       <c r="D58" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="E58" s="13"/>
-      <c r="F58" s="13"/>
-      <c r="G58" s="13"/>
-      <c r="H58" s="13"/>
-      <c r="I58" s="13"/>
-      <c r="J58" s="13"/>
+      <c r="E58" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F58" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="G58" s="13" t="s">
+        <v>281</v>
+      </c>
+      <c r="H58" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="I58" s="13" t="s">
+        <v>283</v>
+      </c>
+      <c r="J58" s="13" t="s">
+        <v>283</v>
+      </c>
       <c r="K58" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:11" ht="72" x14ac:dyDescent="0.3">
       <c r="B59" s="2">
         <v>57</v>
       </c>
@@ -4080,12 +4140,24 @@
       <c r="D59" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="E59" s="13"/>
-      <c r="F59" s="13"/>
-      <c r="G59" s="13"/>
-      <c r="H59" s="13"/>
-      <c r="I59" s="13"/>
-      <c r="J59" s="13"/>
+      <c r="E59" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F59" s="13" t="s">
+        <v>284</v>
+      </c>
+      <c r="G59" s="13" t="s">
+        <v>285</v>
+      </c>
+      <c r="H59" s="13" t="s">
+        <v>286</v>
+      </c>
+      <c r="I59" s="13" t="s">
+        <v>287</v>
+      </c>
+      <c r="J59" s="13" t="s">
+        <v>288</v>
+      </c>
       <c r="K59" s="9" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Added System test cases REQ57-61
</commit_message>
<xml_diff>
--- a/docs/System_Test_Report_template.xlsx
+++ b/docs/System_Test_Report_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E830FC-4CE7-4326-BC00-1CE66BC8138E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6925D68D-C11A-4229-9F41-9E5164E2791D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="306">
   <si>
     <t>Total Test Cases</t>
   </si>
@@ -906,6 +906,57 @@
   </si>
   <si>
     <t>Book shown in database to have no loanadm, reservation or loaned status or date</t>
+  </si>
+  <si>
+    <t>Test that There should also be a general information page showing the number of books that’s on loan, reserved, available books,</t>
+  </si>
+  <si>
+    <t>Website is accessed</t>
+  </si>
+  <si>
+    <t>general information page showing the number of books that’s on loan, reserved, available books is shown</t>
+  </si>
+  <si>
+    <t>Test that Logs should be added, every time an “event” happens, like when a book is returned, loaned or a problem is detected on site, a log is created and should be displayed in a page on the website</t>
+  </si>
+  <si>
+    <t>Open logs is clicked</t>
+  </si>
+  <si>
+    <t>The time, type of log and log msg of every event that has occurred after the RPI is lauched is shown</t>
+  </si>
+  <si>
+    <t>Test that There should be a page for staff to add books into circulation</t>
+  </si>
+  <si>
+    <t>On a browser while connecting to the same network as the RPI, type in the RPI's IP address:5000 then click on the new book button</t>
+  </si>
+  <si>
+    <t>A screen comes up prompting the staff to input book details like id and title and location which is then used to create book on firebase</t>
+  </si>
+  <si>
+    <t>Test that There should be a page for staff to remove books from circulation</t>
+  </si>
+  <si>
+    <t>Bookedit is accessed</t>
+  </si>
+  <si>
+    <t>if updated when red, book will be removed from firebasee</t>
+  </si>
+  <si>
+    <t>Test that There should be a page for staff to remove user accounts</t>
+  </si>
+  <si>
+    <t>User edit is accessed</t>
+  </si>
+  <si>
+    <t>There is a button labeled delete when updating user details, pressing it will cause the screen to toggle red and white, signaling delete or not</t>
+  </si>
+  <si>
+    <t>There is a button labeled delete when updating book details, pressing it will cause the screen to toggle red and white, signaling delete or not</t>
+  </si>
+  <si>
+    <t>if updated when red, user will be removed from firebasee</t>
   </si>
 </sst>
 </file>
@@ -2376,8 +2427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:K128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I58" sqref="I58"/>
+    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4162,7 +4213,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="B60" s="2">
         <v>58</v>
       </c>
@@ -4170,17 +4221,29 @@
       <c r="D60" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="E60" s="13"/>
-      <c r="F60" s="13"/>
-      <c r="G60" s="13"/>
-      <c r="H60" s="13"/>
-      <c r="I60" s="13"/>
-      <c r="J60" s="13"/>
+      <c r="E60" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F60" s="13" t="s">
+        <v>289</v>
+      </c>
+      <c r="G60" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="H60" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="I60" s="13" t="s">
+        <v>291</v>
+      </c>
+      <c r="J60" s="13" t="s">
+        <v>291</v>
+      </c>
       <c r="K60" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B61" s="2">
         <v>59</v>
       </c>
@@ -4188,17 +4251,29 @@
       <c r="D61" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="E61" s="13"/>
-      <c r="F61" s="13"/>
-      <c r="G61" s="13"/>
-      <c r="H61" s="13"/>
-      <c r="I61" s="13"/>
-      <c r="J61" s="13"/>
+      <c r="E61" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F61" s="13" t="s">
+        <v>292</v>
+      </c>
+      <c r="G61" s="13" t="s">
+        <v>293</v>
+      </c>
+      <c r="H61" s="13" t="s">
+        <v>270</v>
+      </c>
+      <c r="I61" s="13" t="s">
+        <v>294</v>
+      </c>
+      <c r="J61" s="13" t="s">
+        <v>294</v>
+      </c>
       <c r="K61" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:11" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B62" s="2">
         <v>60</v>
       </c>
@@ -4206,17 +4281,29 @@
       <c r="D62" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="E62" s="13"/>
-      <c r="F62" s="13"/>
-      <c r="G62" s="13"/>
-      <c r="H62" s="13"/>
-      <c r="I62" s="13"/>
-      <c r="J62" s="13"/>
+      <c r="E62" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F62" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="G62" s="13" t="s">
+        <v>290</v>
+      </c>
+      <c r="H62" s="13" t="s">
+        <v>296</v>
+      </c>
+      <c r="I62" s="13" t="s">
+        <v>297</v>
+      </c>
+      <c r="J62" s="13" t="s">
+        <v>297</v>
+      </c>
       <c r="K62" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:11" ht="72" x14ac:dyDescent="0.3">
       <c r="B63" s="2">
         <v>61</v>
       </c>
@@ -4224,17 +4311,29 @@
       <c r="D63" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="E63" s="13"/>
-      <c r="F63" s="13"/>
-      <c r="G63" s="13"/>
-      <c r="H63" s="13"/>
-      <c r="I63" s="13"/>
-      <c r="J63" s="13"/>
+      <c r="E63" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F63" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="G63" s="13" t="s">
+        <v>299</v>
+      </c>
+      <c r="H63" s="13" t="s">
+        <v>304</v>
+      </c>
+      <c r="I63" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="J63" s="13" t="s">
+        <v>300</v>
+      </c>
       <c r="K63" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:11" ht="72" x14ac:dyDescent="0.3">
       <c r="B64" s="2">
         <v>62</v>
       </c>
@@ -4242,12 +4341,24 @@
       <c r="D64" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="E64" s="13"/>
-      <c r="F64" s="13"/>
-      <c r="G64" s="13"/>
-      <c r="H64" s="13"/>
-      <c r="I64" s="13"/>
-      <c r="J64" s="13"/>
+      <c r="E64" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F64" s="13" t="s">
+        <v>301</v>
+      </c>
+      <c r="G64" s="13" t="s">
+        <v>302</v>
+      </c>
+      <c r="H64" s="13" t="s">
+        <v>303</v>
+      </c>
+      <c r="I64" s="13" t="s">
+        <v>305</v>
+      </c>
+      <c r="J64" s="13" t="s">
+        <v>305</v>
+      </c>
       <c r="K64" s="9" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Added System test cases REQ62-63
</commit_message>
<xml_diff>
--- a/docs/System_Test_Report_template.xlsx
+++ b/docs/System_Test_Report_template.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6925D68D-C11A-4229-9F41-9E5164E2791D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A005F3-9CB6-4C61-A559-B6429E478249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="314">
   <si>
     <t>Total Test Cases</t>
   </si>
@@ -957,6 +957,30 @@
   </si>
   <si>
     <t>if updated when red, user will be removed from firebasee</t>
+  </si>
+  <si>
+    <t>No barcode is scanned for 30 minutes</t>
+  </si>
+  <si>
+    <t>Test that EnterIdle Trigger condition: When no barcode is scanned for 30minute, the Raspberry Pi stops routine DB calls</t>
+  </si>
+  <si>
+    <t>Open the RPI and don’t scan barcodes for 30minutes+- a few minutes</t>
+  </si>
+  <si>
+    <t>Firebase console shows api calls are stagnant</t>
+  </si>
+  <si>
+    <t>Test that EnterAM Trigger condition: When a barcode is scanned while in Idle mode .</t>
+  </si>
+  <si>
+    <t>barcode is scanned in intervals not exceeding 30 minutes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Open the RPI and keep scan barcodes </t>
+  </si>
+  <si>
+    <t>Firebase console shows routine DB calls</t>
   </si>
 </sst>
 </file>
@@ -2428,7 +2452,7 @@
   <dimension ref="B2:K128"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A62" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H63" sqref="H63"/>
+      <selection activeCell="J66" sqref="J66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4363,7 +4387,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:11" ht="72" x14ac:dyDescent="0.3">
       <c r="B65" s="2">
         <v>63</v>
       </c>
@@ -4371,17 +4395,29 @@
       <c r="D65" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="E65" s="13"/>
-      <c r="F65" s="13"/>
-      <c r="G65" s="13"/>
-      <c r="H65" s="13"/>
-      <c r="I65" s="13"/>
-      <c r="J65" s="13"/>
+      <c r="E65" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F65" s="13" t="s">
+        <v>307</v>
+      </c>
+      <c r="G65" s="13" t="s">
+        <v>306</v>
+      </c>
+      <c r="H65" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="I65" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="J65" s="13" t="s">
+        <v>309</v>
+      </c>
       <c r="K65" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:11" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B66" s="2">
         <v>64</v>
       </c>
@@ -4389,12 +4425,24 @@
       <c r="D66" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="E66" s="13"/>
-      <c r="F66" s="13"/>
-      <c r="G66" s="13"/>
-      <c r="H66" s="13"/>
-      <c r="I66" s="13"/>
-      <c r="J66" s="13"/>
+      <c r="E66" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F66" s="13" t="s">
+        <v>310</v>
+      </c>
+      <c r="G66" s="13" t="s">
+        <v>311</v>
+      </c>
+      <c r="H66" s="13" t="s">
+        <v>312</v>
+      </c>
+      <c r="I66" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="J66" s="13" t="s">
+        <v>313</v>
+      </c>
       <c r="K66" s="9" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
Added mode switching add called db function
</commit_message>
<xml_diff>
--- a/docs/System_Test_Report_template.xlsx
+++ b/docs/System_Test_Report_template.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29530"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A005F3-9CB6-4C61-A559-B6429E478249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA433CA9-67CF-4FB0-A104-CE018857E2E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2451,8 +2451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B2:K128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J66" sqref="J66"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H65" sqref="H65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5298,6 +5298,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E81D8C8DDAE8BD44A422697963F06C45" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b6816e004dbb89c674e51f5647972552">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="2b02348f-b4e3-458c-83fc-9e90db0f8029" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e6418ca14ac9ee17b8bbf6df78e0c223" ns2:_="">
     <xsd:import namespace="2b02348f-b4e3-458c-83fc-9e90db0f8029"/>
@@ -5455,22 +5470,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69DB72C7-DF0B-4E18-8174-00AB852E6FB4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2b02348f-b4e3-458c-83fc-9e90db0f8029"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{859B513B-8BED-4B59-B224-E0A2C6173D25}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCDB6385-31B2-4574-9AA4-BF13B563A4E3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5486,28 +5510,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{859B513B-8BED-4B59-B224-E0A2C6173D25}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{69DB72C7-DF0B-4E18-8174-00AB852E6FB4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2b02348f-b4e3-458c-83fc-9e90db0f8029"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>